<commit_message>
[Scene] test cases till #occ006
</commit_message>
<xml_diff>
--- a/car-count-test/car-count-test-cases.xlsx
+++ b/car-count-test/car-count-test-cases.xlsx
@@ -909,10 +909,10 @@
   <dimension ref="A1:G56"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="5" ySplit="2" topLeftCell="F24" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="5" ySplit="2" topLeftCell="F27" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="D37" sqref="D37"/>
+      <selection pane="bottomRight" activeCell="B37" sqref="B37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1447,7 +1447,7 @@
       <c r="A38" t="s">
         <v>88</v>
       </c>
-      <c r="B38" s="5" t="s">
+      <c r="B38" s="11" t="s">
         <v>159</v>
       </c>
       <c r="C38" t="s">

</xml_diff>

<commit_message>
[Scene] test cases till #occ007
</commit_message>
<xml_diff>
--- a/car-count-test/car-count-test-cases.xlsx
+++ b/car-count-test/car-count-test-cases.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="202" uniqueCount="163">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="201" uniqueCount="163">
   <si>
     <t>description</t>
   </si>
@@ -288,13 +288,7 @@
     <t>occ001</t>
   </si>
   <si>
-    <t>discardMatchingBlobs</t>
-  </si>
-  <si>
     <t>car-count test cases</t>
-  </si>
-  <si>
-    <t>discard based on area intersection</t>
   </si>
   <si>
     <t>vel001</t>
@@ -395,9 +389,6 @@
     <t>4 updates necessary</t>
   </si>
   <si>
-    <t>updateTracks</t>
-  </si>
-  <si>
     <t>create new tracks for unassigned blobs</t>
   </si>
   <si>
@@ -489,9 +480,6 @@
     <t>setOcclusion</t>
   </si>
   <si>
-    <t>delete function</t>
-  </si>
-  <si>
     <t>assignBlobsInOcclusion</t>
   </si>
   <si>
@@ -511,6 +499,23 @@
   </si>
   <si>
     <t>based on average velocity</t>
+  </si>
+  <si>
+    <t>updateTracksIntersect</t>
+  </si>
+  <si>
+    <t>one blob -&gt; assign adjusted substitute to track
+two blobs -&gt; regular assign</t>
+  </si>
+  <si>
+    <t>full assignment</t>
+  </si>
+  <si>
+    <t>two blobs moving opposite:
+outside occlusion: assignBlobs
+create occlusion
+inside occlusion: assignBlobsInOcclusion
+delete occlusion</t>
   </si>
 </sst>
 </file>
@@ -548,7 +553,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -558,12 +563,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="6" tint="0.79998168889431442"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -580,7 +579,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -601,10 +600,6 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -906,13 +901,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G56"/>
+  <dimension ref="A1:G55"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="5" ySplit="2" topLeftCell="F27" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="B37" sqref="B37"/>
+      <selection pane="bottomRight" activeCell="E40" sqref="E40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -927,7 +922,7 @@
   <sheetData>
     <row r="1" spans="1:7" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D1" s="9" t="s">
         <v>68</v>
@@ -1124,7 +1119,7 @@
         <v>85</v>
       </c>
       <c r="C14" s="8" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
@@ -1132,13 +1127,13 @@
         <v>87</v>
       </c>
       <c r="B16" s="5" t="s">
+        <v>99</v>
+      </c>
+      <c r="C16" t="s">
+        <v>100</v>
+      </c>
+      <c r="D16" t="s">
         <v>101</v>
-      </c>
-      <c r="C16" t="s">
-        <v>102</v>
-      </c>
-      <c r="D16" t="s">
-        <v>103</v>
       </c>
     </row>
     <row r="17" spans="1:5" ht="30" x14ac:dyDescent="0.25">
@@ -1146,16 +1141,16 @@
         <v>87</v>
       </c>
       <c r="B17" s="5" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="C17" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="D17" s="8" t="s">
+        <v>102</v>
+      </c>
+      <c r="E17" s="8" t="s">
         <v>104</v>
-      </c>
-      <c r="E17" s="8" t="s">
-        <v>106</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
@@ -1163,16 +1158,16 @@
         <v>87</v>
       </c>
       <c r="B18" s="5" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="C18" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="D18" s="8" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="E18" s="8" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
     </row>
     <row r="19" spans="1:5" ht="30" x14ac:dyDescent="0.25">
@@ -1180,16 +1175,16 @@
         <v>87</v>
       </c>
       <c r="B19" s="5" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="C19" t="s">
+        <v>116</v>
+      </c>
+      <c r="D19" s="8" t="s">
         <v>118</v>
       </c>
-      <c r="D19" s="8" t="s">
-        <v>120</v>
-      </c>
       <c r="E19" s="8" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
@@ -1197,16 +1192,16 @@
         <v>87</v>
       </c>
       <c r="B20" s="5" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="C20" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="D20" s="8" t="s">
+        <v>141</v>
+      </c>
+      <c r="E20" s="8" t="s">
         <v>144</v>
-      </c>
-      <c r="E20" s="8" t="s">
-        <v>147</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
@@ -1214,16 +1209,16 @@
         <v>87</v>
       </c>
       <c r="B21" s="5" t="s">
+        <v>107</v>
+      </c>
+      <c r="C21" t="s">
+        <v>96</v>
+      </c>
+      <c r="D21" s="8" t="s">
+        <v>108</v>
+      </c>
+      <c r="E21" s="8" t="s">
         <v>109</v>
-      </c>
-      <c r="C21" t="s">
-        <v>98</v>
-      </c>
-      <c r="D21" s="8" t="s">
-        <v>110</v>
-      </c>
-      <c r="E21" s="8" t="s">
-        <v>111</v>
       </c>
     </row>
     <row r="22" spans="1:5" ht="30" x14ac:dyDescent="0.25">
@@ -1231,16 +1226,16 @@
         <v>87</v>
       </c>
       <c r="B22" s="5" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="C22" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="D22" s="8" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="E22" s="8" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
@@ -1248,16 +1243,16 @@
         <v>87</v>
       </c>
       <c r="B23" s="5" t="s">
+        <v>113</v>
+      </c>
+      <c r="C23" t="s">
+        <v>96</v>
+      </c>
+      <c r="D23" s="8" t="s">
+        <v>114</v>
+      </c>
+      <c r="E23" s="8" t="s">
         <v>115</v>
-      </c>
-      <c r="C23" t="s">
-        <v>98</v>
-      </c>
-      <c r="D23" s="8" t="s">
-        <v>116</v>
-      </c>
-      <c r="E23" s="8" t="s">
-        <v>117</v>
       </c>
     </row>
     <row r="24" spans="1:5" ht="30" x14ac:dyDescent="0.25">
@@ -1265,16 +1260,16 @@
         <v>87</v>
       </c>
       <c r="B24" s="5" t="s">
+        <v>119</v>
+      </c>
+      <c r="C24" t="s">
+        <v>97</v>
+      </c>
+      <c r="D24" s="8" t="s">
+        <v>120</v>
+      </c>
+      <c r="E24" s="8" t="s">
         <v>121</v>
-      </c>
-      <c r="C24" t="s">
-        <v>99</v>
-      </c>
-      <c r="D24" s="8" t="s">
-        <v>122</v>
-      </c>
-      <c r="E24" s="8" t="s">
-        <v>123</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
@@ -1285,10 +1280,10 @@
         <v>88</v>
       </c>
       <c r="B27" s="5" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="C27" s="8" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
@@ -1296,16 +1291,16 @@
         <v>88</v>
       </c>
       <c r="B28" s="5" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="C28" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="D28" s="8" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="E28" s="8" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
     </row>
     <row r="29" spans="1:5" ht="30" x14ac:dyDescent="0.25">
@@ -1313,16 +1308,16 @@
         <v>88</v>
       </c>
       <c r="B29" s="5" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="C29" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="D29" s="8" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="E29" s="8" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
@@ -1330,13 +1325,13 @@
         <v>88</v>
       </c>
       <c r="B30" s="5" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="C30" t="s">
+        <v>136</v>
+      </c>
+      <c r="D30" s="8" t="s">
         <v>139</v>
-      </c>
-      <c r="D30" s="8" t="s">
-        <v>142</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
@@ -1344,13 +1339,13 @@
         <v>88</v>
       </c>
       <c r="B31" s="5" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="C31" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="D31" s="8" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
@@ -1361,13 +1356,13 @@
         <v>89</v>
       </c>
       <c r="C32" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="D32" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="E32" s="8" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.25">
@@ -1375,13 +1370,13 @@
         <v>88</v>
       </c>
       <c r="B33" s="5" t="s">
+        <v>127</v>
+      </c>
+      <c r="C33" t="s">
+        <v>126</v>
+      </c>
+      <c r="D33" t="s">
         <v>130</v>
-      </c>
-      <c r="C33" t="s">
-        <v>129</v>
-      </c>
-      <c r="D33" t="s">
-        <v>133</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.25">
@@ -1389,13 +1384,13 @@
         <v>88</v>
       </c>
       <c r="B34" s="5" t="s">
+        <v>128</v>
+      </c>
+      <c r="C34" t="s">
+        <v>129</v>
+      </c>
+      <c r="D34" t="s">
         <v>131</v>
-      </c>
-      <c r="C34" t="s">
-        <v>132</v>
-      </c>
-      <c r="D34" t="s">
-        <v>134</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.25">
@@ -1403,16 +1398,16 @@
         <v>88</v>
       </c>
       <c r="B35" s="5" t="s">
+        <v>148</v>
+      </c>
+      <c r="C35" t="s">
         <v>151</v>
       </c>
-      <c r="C35" t="s">
-        <v>154</v>
-      </c>
       <c r="D35" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="E35" s="8" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.25">
@@ -1420,13 +1415,13 @@
         <v>88</v>
       </c>
       <c r="B36" s="5" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="C36" t="s">
-        <v>157</v>
+        <v>153</v>
       </c>
       <c r="D36" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.25">
@@ -1434,50 +1429,58 @@
         <v>88</v>
       </c>
       <c r="B37" s="5" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
       <c r="C37" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
       <c r="D37" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>88</v>
       </c>
-      <c r="B38" s="11" t="s">
+      <c r="B38" s="5" t="s">
+        <v>155</v>
+      </c>
+      <c r="C38" t="s">
+        <v>152</v>
+      </c>
+      <c r="D38" s="8" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" ht="75" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>88</v>
+      </c>
+      <c r="B39" t="s">
+        <v>107</v>
+      </c>
+      <c r="C39" t="s">
         <v>159</v>
       </c>
-      <c r="C38" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="39" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A39" s="12" t="s">
-        <v>88</v>
-      </c>
-      <c r="B39" s="12" t="s">
-        <v>155</v>
-      </c>
-      <c r="C39" s="12" t="s">
-        <v>90</v>
-      </c>
-      <c r="D39" s="13" t="s">
-        <v>92</v>
-      </c>
-      <c r="E39" s="13"/>
-    </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A40" t="s">
-        <v>88</v>
-      </c>
-      <c r="B40" t="s">
-        <v>109</v>
-      </c>
-      <c r="C40" t="s">
-        <v>124</v>
+      <c r="D39" t="s">
+        <v>161</v>
+      </c>
+      <c r="E39" s="8" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C47" t="s">
+        <v>3</v>
+      </c>
+      <c r="D47" t="s">
+        <v>4</v>
+      </c>
+      <c r="E47" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="F47" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.25">
@@ -1485,13 +1488,10 @@
         <v>3</v>
       </c>
       <c r="D48" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="E48" s="8" t="s">
-        <v>8</v>
-      </c>
-      <c r="F48" t="s">
-        <v>19</v>
+        <v>9</v>
       </c>
     </row>
     <row r="49" spans="3:6" x14ac:dyDescent="0.25">
@@ -1499,45 +1499,34 @@
         <v>3</v>
       </c>
       <c r="D49" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="E49" s="8" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="50" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C50" t="s">
-        <v>3</v>
-      </c>
-      <c r="D50" t="s">
-        <v>6</v>
-      </c>
-      <c r="E50" s="8" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="52" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C52" t="s">
+    <row r="51" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C51" t="s">
         <v>13</v>
       </c>
-      <c r="D52" t="s">
+      <c r="D51" t="s">
         <v>14</v>
       </c>
-      <c r="E52" s="8" t="s">
+      <c r="E51" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="F52" t="s">
+      <c r="F51" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="56" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C56" t="s">
+    <row r="55" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C55" t="s">
         <v>16</v>
       </c>
-      <c r="E56" s="8" t="s">
+      <c r="E55" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="F56" t="s">
+      <c r="F55" t="s">
         <v>21</v>
       </c>
     </row>

</xml_diff>

<commit_message>
[Scene] test cases fished up to #upd001
</commit_message>
<xml_diff>
--- a/car-count-test/car-count-test-cases.xlsx
+++ b/car-count-test/car-count-test-cases.xlsx
@@ -904,10 +904,10 @@
   <dimension ref="A1:G55"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="5" ySplit="2" topLeftCell="F27" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="5" ySplit="2" topLeftCell="F33" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="E40" sqref="E40"/>
+      <selection pane="bottomRight" activeCell="D34" sqref="D34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1456,7 +1456,7 @@
       <c r="A39" t="s">
         <v>88</v>
       </c>
-      <c r="B39" t="s">
+      <c r="B39" s="5" t="s">
         <v>107</v>
       </c>
       <c r="C39" t="s">

</xml_diff>

<commit_message>
fix #16 delete occlusion, if at least one track was deleted
</commit_message>
<xml_diff>
--- a/car-count-test/car-count-test-cases.xlsx
+++ b/car-count-test/car-count-test-cases.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="201" uniqueCount="163">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="210" uniqueCount="168">
   <si>
     <t>description</t>
   </si>
@@ -365,9 +365,6 @@
   </si>
   <si>
     <t>confidence in- / decrease</t>
-  </si>
-  <si>
-    <t>marked for deletion, if conf drops below 0</t>
   </si>
   <si>
     <t>addSubstitute</t>
@@ -516,6 +513,24 @@
 create occlusion
 inside occlusion: assignBlobsInOcclusion
 delete occlusion</t>
+  </si>
+  <si>
+    <t>mark for deletion, if conf drops below 0</t>
+  </si>
+  <si>
+    <t>upd005</t>
+  </si>
+  <si>
+    <t>mark for deletion, if substitute outside roi</t>
+  </si>
+  <si>
+    <t xml:space="preserve">delete tracks outside roi </t>
+  </si>
+  <si>
+    <t>occ008</t>
+  </si>
+  <si>
+    <t>delete occlusion, if one of the tracks have been deleted</t>
   </si>
 </sst>
 </file>
@@ -901,13 +916,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G55"/>
+  <dimension ref="A1:G56"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="5" ySplit="2" topLeftCell="F33" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="5" ySplit="2" topLeftCell="F27" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="D34" sqref="D34"/>
+      <selection pane="bottomRight" activeCell="D40" sqref="D40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1178,13 +1193,13 @@
         <v>98</v>
       </c>
       <c r="C19" t="s">
+        <v>115</v>
+      </c>
+      <c r="D19" s="8" t="s">
+        <v>117</v>
+      </c>
+      <c r="E19" s="8" t="s">
         <v>116</v>
-      </c>
-      <c r="D19" s="8" t="s">
-        <v>118</v>
-      </c>
-      <c r="E19" s="8" t="s">
-        <v>117</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
@@ -1192,16 +1207,16 @@
         <v>87</v>
       </c>
       <c r="B20" s="5" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="C20" t="s">
+        <v>139</v>
+      </c>
+      <c r="D20" s="8" t="s">
         <v>140</v>
       </c>
-      <c r="D20" s="8" t="s">
-        <v>141</v>
-      </c>
       <c r="E20" s="8" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
@@ -1252,7 +1267,7 @@
         <v>114</v>
       </c>
       <c r="E23" s="8" t="s">
-        <v>115</v>
+        <v>162</v>
       </c>
     </row>
     <row r="24" spans="1:5" ht="30" x14ac:dyDescent="0.25">
@@ -1260,16 +1275,33 @@
         <v>87</v>
       </c>
       <c r="B24" s="5" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C24" t="s">
         <v>97</v>
       </c>
       <c r="D24" s="8" t="s">
+        <v>119</v>
+      </c>
+      <c r="E24" s="8" t="s">
         <v>120</v>
       </c>
-      <c r="E24" s="8" t="s">
-        <v>121</v>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>87</v>
+      </c>
+      <c r="B25" s="5" t="s">
+        <v>163</v>
+      </c>
+      <c r="C25" t="s">
+        <v>96</v>
+      </c>
+      <c r="D25" s="8" t="s">
+        <v>165</v>
+      </c>
+      <c r="E25" s="8" t="s">
+        <v>164</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
@@ -1283,7 +1315,7 @@
         <v>99</v>
       </c>
       <c r="C27" s="8" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
@@ -1297,10 +1329,10 @@
         <v>94</v>
       </c>
       <c r="D28" s="8" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="E28" s="8" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="29" spans="1:5" ht="30" x14ac:dyDescent="0.25">
@@ -1308,16 +1340,16 @@
         <v>88</v>
       </c>
       <c r="B29" s="5" t="s">
+        <v>132</v>
+      </c>
+      <c r="C29" t="s">
         <v>133</v>
       </c>
-      <c r="C29" t="s">
-        <v>134</v>
-      </c>
       <c r="D29" s="8" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="E29" s="8" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
@@ -1325,13 +1357,13 @@
         <v>88</v>
       </c>
       <c r="B30" s="5" t="s">
+        <v>134</v>
+      </c>
+      <c r="C30" t="s">
         <v>135</v>
       </c>
-      <c r="C30" t="s">
-        <v>136</v>
-      </c>
       <c r="D30" s="8" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
@@ -1339,13 +1371,13 @@
         <v>88</v>
       </c>
       <c r="B31" s="5" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="C31" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="D31" s="8" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
@@ -1356,13 +1388,13 @@
         <v>89</v>
       </c>
       <c r="C32" t="s">
+        <v>122</v>
+      </c>
+      <c r="D32" t="s">
         <v>123</v>
       </c>
-      <c r="D32" t="s">
+      <c r="E32" s="8" t="s">
         <v>124</v>
-      </c>
-      <c r="E32" s="8" t="s">
-        <v>125</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.25">
@@ -1370,13 +1402,13 @@
         <v>88</v>
       </c>
       <c r="B33" s="5" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C33" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="D33" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.25">
@@ -1384,13 +1416,13 @@
         <v>88</v>
       </c>
       <c r="B34" s="5" t="s">
+        <v>127</v>
+      </c>
+      <c r="C34" t="s">
         <v>128</v>
       </c>
-      <c r="C34" t="s">
-        <v>129</v>
-      </c>
       <c r="D34" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.25">
@@ -1398,16 +1430,16 @@
         <v>88</v>
       </c>
       <c r="B35" s="5" t="s">
+        <v>147</v>
+      </c>
+      <c r="C35" t="s">
+        <v>150</v>
+      </c>
+      <c r="D35" t="s">
         <v>148</v>
       </c>
-      <c r="C35" t="s">
-        <v>151</v>
-      </c>
-      <c r="D35" t="s">
+      <c r="E35" s="8" t="s">
         <v>149</v>
-      </c>
-      <c r="E35" s="8" t="s">
-        <v>150</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.25">
@@ -1415,13 +1447,13 @@
         <v>88</v>
       </c>
       <c r="B36" s="5" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C36" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="D36" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.25">
@@ -1429,13 +1461,13 @@
         <v>88</v>
       </c>
       <c r="B37" s="5" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="C37" t="s">
+        <v>155</v>
+      </c>
+      <c r="D37" t="s">
         <v>156</v>
-      </c>
-      <c r="D37" t="s">
-        <v>157</v>
       </c>
     </row>
     <row r="38" spans="1:6" ht="45" x14ac:dyDescent="0.25">
@@ -1443,44 +1475,44 @@
         <v>88</v>
       </c>
       <c r="B38" s="5" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="C38" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="D38" s="8" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="39" spans="1:6" ht="75" x14ac:dyDescent="0.25">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>88</v>
       </c>
-      <c r="B39" s="5" t="s">
+      <c r="B39" s="11" t="s">
+        <v>166</v>
+      </c>
+      <c r="C39" t="s">
+        <v>151</v>
+      </c>
+      <c r="D39" s="8" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" ht="75" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>88</v>
+      </c>
+      <c r="B40" s="5" t="s">
         <v>107</v>
       </c>
-      <c r="C39" t="s">
-        <v>159</v>
-      </c>
-      <c r="D39" t="s">
+      <c r="C40" t="s">
+        <v>158</v>
+      </c>
+      <c r="D40" t="s">
+        <v>160</v>
+      </c>
+      <c r="E40" s="8" t="s">
         <v>161</v>
-      </c>
-      <c r="E39" s="8" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="C47" t="s">
-        <v>3</v>
-      </c>
-      <c r="D47" t="s">
-        <v>4</v>
-      </c>
-      <c r="E47" s="8" t="s">
-        <v>8</v>
-      </c>
-      <c r="F47" t="s">
-        <v>19</v>
       </c>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.25">
@@ -1488,10 +1520,13 @@
         <v>3</v>
       </c>
       <c r="D48" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E48" s="8" t="s">
-        <v>9</v>
+        <v>8</v>
+      </c>
+      <c r="F48" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="49" spans="3:6" x14ac:dyDescent="0.25">
@@ -1499,34 +1534,45 @@
         <v>3</v>
       </c>
       <c r="D49" t="s">
+        <v>5</v>
+      </c>
+      <c r="E49" s="8" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="50" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C50" t="s">
+        <v>3</v>
+      </c>
+      <c r="D50" t="s">
         <v>6</v>
       </c>
-      <c r="E49" s="8" t="s">
+      <c r="E50" s="8" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="51" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C51" t="s">
+    <row r="52" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C52" t="s">
         <v>13</v>
       </c>
-      <c r="D51" t="s">
+      <c r="D52" t="s">
         <v>14</v>
       </c>
-      <c r="E51" s="8" t="s">
+      <c r="E52" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="F51" t="s">
+      <c r="F52" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="55" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C55" t="s">
+    <row r="56" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C56" t="s">
         <v>16</v>
       </c>
-      <c r="E55" s="8" t="s">
+      <c r="E56" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="F55" t="s">
+      <c r="F56" t="s">
         <v>21</v>
       </c>
     </row>

</xml_diff>

<commit_message>
msvc-car-count-test started, test cases defined in xls
</commit_message>
<xml_diff>
--- a/car-count-test/car-count-test-cases.xlsx
+++ b/car-count-test/car-count-test-cases.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="219" uniqueCount="174">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="259" uniqueCount="196">
   <si>
     <t>description</t>
   </si>
@@ -455,10 +455,6 @@
     <t>no change within backlash</t>
   </si>
   <si>
-    <t>getTrackID
-returnTrackID</t>
-  </si>
-  <si>
     <t>keep track with longer history</t>
   </si>
   <si>
@@ -477,16 +473,10 @@
     <t>setOcclusion</t>
   </si>
   <si>
-    <t>assignBlobsInOcclusion</t>
-  </si>
-  <si>
     <t>calcSubstitute</t>
   </si>
   <si>
     <t>occ006</t>
-  </si>
-  <si>
-    <t>occ007</t>
   </si>
   <si>
     <t>adjustSubstPos</t>
@@ -530,25 +520,100 @@
     <t>occ008</t>
   </si>
   <si>
-    <t>delete occlusion, if one of the tracks have been deleted</t>
-  </si>
-  <si>
-    <t>pullID</t>
-  </si>
-  <si>
     <t>[Occlusion]</t>
   </si>
   <si>
-    <t>c'tor, copy c'tor</t>
-  </si>
-  <si>
-    <t>returnID</t>
-  </si>
-  <si>
-    <t>d'tor</t>
-  </si>
-  <si>
     <t>refactor to base class UniqueID</t>
+  </si>
+  <si>
+    <t>[fcn-track]</t>
+  </si>
+  <si>
+    <t>del003</t>
+  </si>
+  <si>
+    <t>deleteOcclusionWithMarkedTracks</t>
+  </si>
+  <si>
+    <t>cnt001</t>
+  </si>
+  <si>
+    <t>countVehicles</t>
+  </si>
+  <si>
+    <t>id002</t>
+  </si>
+  <si>
+    <t>id</t>
+  </si>
+  <si>
+    <t>updateRect</t>
+  </si>
+  <si>
+    <t>change occlusion rect based on track rects</t>
+  </si>
+  <si>
+    <t>pas001</t>
+  </si>
+  <si>
+    <t>hasPassed</t>
+  </si>
+  <si>
+    <t>con001</t>
+  </si>
+  <si>
+    <t>constructor</t>
+  </si>
+  <si>
+    <t>[OcclusionIdList]</t>
+  </si>
+  <si>
+    <t>add001</t>
+  </si>
+  <si>
+    <t>addOcclusion</t>
+  </si>
+  <si>
+    <t>getList</t>
+  </si>
+  <si>
+    <t>isOcclusion</t>
+  </si>
+  <si>
+    <t>remove</t>
+  </si>
+  <si>
+    <t>get001</t>
+  </si>
+  <si>
+    <t>rem001</t>
+  </si>
+  <si>
+    <t>returnTrackID</t>
+  </si>
+  <si>
+    <t>getTrackID</t>
+  </si>
+  <si>
+    <t>occlusionList</t>
+  </si>
+  <si>
+    <t>obs001</t>
+  </si>
+  <si>
+    <t>update</t>
+  </si>
+  <si>
+    <t>update observer</t>
+  </si>
+  <si>
+    <t>delete, if one track is marked for deletion</t>
+  </si>
+  <si>
+    <t>status: has to be changed</t>
+  </si>
+  <si>
+    <t>setID</t>
   </si>
 </sst>
 </file>
@@ -593,7 +658,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -612,8 +677,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -621,11 +692,20 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -642,20 +722,36 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
+  <colors>
+    <mruColors>
+      <color rgb="FFFFFF99"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -951,22 +1047,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G60"/>
+  <dimension ref="A1:G75"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="5" ySplit="2" topLeftCell="F25" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="5" ySplit="2" topLeftCell="F17" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="B41" sqref="B41"/>
+      <selection pane="bottomRight" activeCell="C29" sqref="C29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.7109375" customWidth="1"/>
+    <col min="1" max="1" width="17.140625" customWidth="1"/>
     <col min="2" max="2" width="12.42578125" customWidth="1"/>
-    <col min="3" max="3" width="19.7109375" customWidth="1"/>
-    <col min="4" max="4" width="28" customWidth="1"/>
-    <col min="5" max="5" width="41.85546875" style="8" customWidth="1"/>
+    <col min="3" max="3" width="31.7109375" customWidth="1"/>
+    <col min="4" max="4" width="42.28515625" customWidth="1"/>
+    <col min="5" max="5" width="50.42578125" style="8" customWidth="1"/>
     <col min="6" max="6" width="25.28515625" customWidth="1"/>
     <col min="7" max="7" width="45.140625" customWidth="1"/>
   </cols>
@@ -978,7 +1074,10 @@
       <c r="D1" s="9" t="s">
         <v>68</v>
       </c>
-      <c r="E1" s="10" t="s">
+      <c r="E1" s="19" t="s">
+        <v>194</v>
+      </c>
+      <c r="F1" s="20" t="s">
         <v>69</v>
       </c>
     </row>
@@ -1105,7 +1204,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
         <v>81</v>
       </c>
@@ -1124,16 +1223,17 @@
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="3"/>
-      <c r="B10" s="11"/>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A11" s="3" t="s">
+      <c r="B10" s="10"/>
+    </row>
+    <row r="11" spans="1:7" s="16" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="14" t="s">
         <v>82</v>
       </c>
-      <c r="B11" s="5" t="s">
+      <c r="B11" s="15" t="s">
         <v>78</v>
       </c>
-      <c r="F11" t="s">
+      <c r="E11" s="17"/>
+      <c r="F11" s="16" t="s">
         <v>74</v>
       </c>
     </row>
@@ -1173,19 +1273,20 @@
         <v>103</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
+    <row r="16" spans="1:7" s="16" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="16" t="s">
         <v>87</v>
       </c>
-      <c r="B16" s="5" t="s">
+      <c r="B16" s="15" t="s">
         <v>99</v>
       </c>
-      <c r="C16" t="s">
+      <c r="C16" s="16" t="s">
         <v>100</v>
       </c>
-      <c r="D16" t="s">
+      <c r="D16" s="16" t="s">
         <v>101</v>
       </c>
+      <c r="E16" s="17"/>
     </row>
     <row r="17" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
@@ -1303,7 +1404,7 @@
         <v>114</v>
       </c>
       <c r="E23" s="8" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
     </row>
     <row r="24" spans="1:5" ht="30" x14ac:dyDescent="0.25">
@@ -1328,322 +1429,488 @@
         <v>87</v>
       </c>
       <c r="B25" s="5" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="C25" t="s">
         <v>96</v>
       </c>
       <c r="D25" s="8" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="E25" s="8" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B26" s="10"/>
+      <c r="D26" s="8"/>
+    </row>
+    <row r="27" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
         <v>164</v>
       </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B26" s="5"/>
-      <c r="D26" s="8"/>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
-        <v>169</v>
-      </c>
-      <c r="B27" s="5" t="s">
-        <v>99</v>
+      <c r="B27" s="12" t="s">
+        <v>95</v>
       </c>
       <c r="C27" t="s">
-        <v>168</v>
+        <v>94</v>
       </c>
       <c r="D27" s="8" t="s">
-        <v>170</v>
-      </c>
-      <c r="E27" s="12" t="s">
-        <v>173</v>
+        <v>156</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>169</v>
+        <v>164</v>
       </c>
       <c r="B28" s="5" t="s">
         <v>99</v>
       </c>
       <c r="C28" t="s">
+        <v>172</v>
+      </c>
+      <c r="D28" s="8"/>
+      <c r="E28" s="11" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>164</v>
+      </c>
+      <c r="B29" s="5" t="s">
         <v>171</v>
       </c>
-      <c r="D28" s="8" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C29" t="s">
+        <v>195</v>
+      </c>
       <c r="D29" s="8"/>
-    </row>
-    <row r="30" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="E29" s="11"/>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>88</v>
-      </c>
-      <c r="B30" s="5" t="s">
-        <v>99</v>
-      </c>
-      <c r="C30" s="8" t="s">
-        <v>144</v>
-      </c>
+        <v>164</v>
+      </c>
+      <c r="B30" s="12" t="s">
+        <v>175</v>
+      </c>
+      <c r="C30" t="s">
+        <v>176</v>
+      </c>
+      <c r="D30" s="8"/>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>88</v>
-      </c>
-      <c r="B31" s="5" t="s">
-        <v>95</v>
+        <v>164</v>
+      </c>
+      <c r="B31" s="12" t="s">
+        <v>107</v>
       </c>
       <c r="C31" t="s">
-        <v>94</v>
+        <v>173</v>
       </c>
       <c r="D31" s="8" t="s">
-        <v>142</v>
-      </c>
-      <c r="E31" s="8" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A32" t="s">
-        <v>88</v>
-      </c>
-      <c r="B32" s="5" t="s">
-        <v>132</v>
-      </c>
-      <c r="C32" t="s">
-        <v>133</v>
-      </c>
-      <c r="D32" s="8" t="s">
-        <v>137</v>
-      </c>
-      <c r="E32" s="8" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A33" t="s">
-        <v>88</v>
-      </c>
-      <c r="B33" s="5" t="s">
-        <v>134</v>
-      </c>
-      <c r="C33" t="s">
-        <v>135</v>
-      </c>
-      <c r="D33" s="8" t="s">
-        <v>138</v>
-      </c>
+        <v>174</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B32" s="10"/>
+      <c r="D32" s="8"/>
+    </row>
+    <row r="33" spans="1:5" s="16" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="16" t="s">
+        <v>179</v>
+      </c>
+      <c r="B33" s="18" t="s">
+        <v>177</v>
+      </c>
+      <c r="C33" s="16" t="s">
+        <v>178</v>
+      </c>
+      <c r="D33" s="17"/>
+      <c r="E33" s="17"/>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>88</v>
-      </c>
-      <c r="B34" s="5" t="s">
-        <v>136</v>
+        <v>179</v>
+      </c>
+      <c r="B34" s="12" t="s">
+        <v>180</v>
       </c>
       <c r="C34" t="s">
-        <v>146</v>
-      </c>
-      <c r="D34" s="8" t="s">
-        <v>138</v>
-      </c>
+        <v>181</v>
+      </c>
+      <c r="D34" s="8"/>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>88</v>
-      </c>
-      <c r="B35" s="5" t="s">
-        <v>89</v>
+        <v>179</v>
+      </c>
+      <c r="B35" s="12" t="s">
+        <v>95</v>
       </c>
       <c r="C35" t="s">
-        <v>122</v>
-      </c>
-      <c r="D35" t="s">
-        <v>123</v>
-      </c>
-      <c r="E35" s="8" t="s">
-        <v>124</v>
-      </c>
+        <v>94</v>
+      </c>
+      <c r="D35" s="8"/>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>88</v>
-      </c>
-      <c r="B36" s="5" t="s">
-        <v>126</v>
+        <v>179</v>
+      </c>
+      <c r="B36" s="12" t="s">
+        <v>185</v>
       </c>
       <c r="C36" t="s">
-        <v>125</v>
-      </c>
-      <c r="D36" t="s">
-        <v>129</v>
-      </c>
+        <v>182</v>
+      </c>
+      <c r="D36" s="8"/>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>88</v>
-      </c>
-      <c r="B37" s="5" t="s">
-        <v>127</v>
+        <v>179</v>
+      </c>
+      <c r="B37" s="12" t="s">
+        <v>89</v>
       </c>
       <c r="C37" t="s">
-        <v>128</v>
-      </c>
-      <c r="D37" t="s">
-        <v>130</v>
-      </c>
+        <v>183</v>
+      </c>
+      <c r="D37" s="8"/>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
+        <v>179</v>
+      </c>
+      <c r="B38" s="12" t="s">
+        <v>186</v>
+      </c>
+      <c r="C38" t="s">
+        <v>184</v>
+      </c>
+      <c r="D38" s="8"/>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D39" s="8"/>
+    </row>
+    <row r="40" spans="1:5" s="16" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A40" s="16" t="s">
         <v>88</v>
       </c>
-      <c r="B38" s="5" t="s">
-        <v>147</v>
-      </c>
-      <c r="C38" t="s">
-        <v>150</v>
-      </c>
-      <c r="D38" t="s">
-        <v>148</v>
-      </c>
-      <c r="E38" s="8" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A39" t="s">
-        <v>88</v>
-      </c>
-      <c r="B39" s="5" t="s">
-        <v>131</v>
-      </c>
-      <c r="C39" t="s">
-        <v>152</v>
-      </c>
-      <c r="D39" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A40" t="s">
-        <v>88</v>
-      </c>
-      <c r="B40" s="5" t="s">
-        <v>153</v>
-      </c>
-      <c r="C40" t="s">
-        <v>155</v>
-      </c>
-      <c r="D40" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="41" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="B40" s="18" t="s">
+        <v>177</v>
+      </c>
+      <c r="C40" s="16" t="s">
+        <v>178</v>
+      </c>
+      <c r="D40" s="17"/>
+      <c r="E40" s="17"/>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>88</v>
       </c>
       <c r="B41" s="13" t="s">
-        <v>154</v>
+        <v>95</v>
       </c>
       <c r="C41" t="s">
-        <v>151</v>
+        <v>94</v>
       </c>
       <c r="D41" s="8" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="42" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+        <v>142</v>
+      </c>
+      <c r="E41" s="8" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>88</v>
       </c>
-      <c r="B42" s="11" t="s">
-        <v>166</v>
+      <c r="B42" s="12" t="s">
+        <v>169</v>
       </c>
       <c r="C42" t="s">
-        <v>151</v>
-      </c>
-      <c r="D42" s="8" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="44" spans="1:5" ht="75" x14ac:dyDescent="0.25">
+        <v>170</v>
+      </c>
+      <c r="D42" s="8"/>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>88</v>
+      </c>
+      <c r="B43" s="5" t="s">
+        <v>134</v>
+      </c>
+      <c r="C43" t="s">
+        <v>135</v>
+      </c>
+      <c r="D43" s="8" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>88</v>
       </c>
       <c r="B44" s="5" t="s">
+        <v>167</v>
+      </c>
+      <c r="C44" t="s">
+        <v>168</v>
+      </c>
+      <c r="D44" s="8" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>88</v>
+      </c>
+      <c r="B45" s="5" t="s">
+        <v>136</v>
+      </c>
+      <c r="C45" t="s">
+        <v>145</v>
+      </c>
+      <c r="D45" s="8" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>88</v>
+      </c>
+      <c r="B46" s="5" t="s">
+        <v>99</v>
+      </c>
+      <c r="C46" s="8" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>88</v>
+      </c>
+      <c r="B47" s="12" t="s">
+        <v>163</v>
+      </c>
+      <c r="C47" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>88</v>
+      </c>
+      <c r="B48" s="5" t="s">
+        <v>171</v>
+      </c>
+      <c r="C48" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
+        <v>88</v>
+      </c>
+      <c r="B49" s="5" t="s">
+        <v>146</v>
+      </c>
+      <c r="C49" t="s">
+        <v>149</v>
+      </c>
+      <c r="D49" t="s">
+        <v>147</v>
+      </c>
+      <c r="E49" s="8" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>88</v>
+      </c>
+      <c r="B50" s="5" t="s">
+        <v>190</v>
+      </c>
+      <c r="C50" t="s">
+        <v>191</v>
+      </c>
+      <c r="D50" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" ht="75" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>88</v>
+      </c>
+      <c r="B51" s="5" t="s">
         <v>107</v>
       </c>
-      <c r="C44" t="s">
+      <c r="C51" t="s">
+        <v>155</v>
+      </c>
+      <c r="D51" t="s">
+        <v>157</v>
+      </c>
+      <c r="E51" s="8" t="s">
         <v>158</v>
       </c>
-      <c r="D44" t="s">
-        <v>160</v>
-      </c>
-      <c r="E44" s="8" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="52" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C52" t="s">
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B52" s="10"/>
+      <c r="D52" s="8"/>
+    </row>
+    <row r="53" spans="1:5" s="16" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A53" s="16" t="s">
+        <v>166</v>
+      </c>
+      <c r="B53" s="15" t="s">
+        <v>151</v>
+      </c>
+      <c r="C53" s="16" t="s">
+        <v>152</v>
+      </c>
+      <c r="D53" s="16" t="s">
+        <v>153</v>
+      </c>
+      <c r="E53" s="17"/>
+    </row>
+    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
+        <v>166</v>
+      </c>
+      <c r="B54" s="5" t="s">
+        <v>131</v>
+      </c>
+      <c r="C54" t="s">
+        <v>150</v>
+      </c>
+      <c r="D54" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
+        <v>166</v>
+      </c>
+      <c r="B55" s="5" t="s">
+        <v>132</v>
+      </c>
+      <c r="C55" t="s">
+        <v>133</v>
+      </c>
+      <c r="D55" s="8" t="s">
+        <v>137</v>
+      </c>
+      <c r="E55" s="8" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A56" t="s">
+        <v>166</v>
+      </c>
+      <c r="B56" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="C56" t="s">
+        <v>122</v>
+      </c>
+      <c r="D56" t="s">
+        <v>123</v>
+      </c>
+      <c r="E56" s="8" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A57" t="s">
+        <v>166</v>
+      </c>
+      <c r="B57" s="5" t="s">
+        <v>126</v>
+      </c>
+      <c r="C57" t="s">
+        <v>125</v>
+      </c>
+      <c r="D57" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A58" t="s">
+        <v>166</v>
+      </c>
+      <c r="B58" s="5" t="s">
+        <v>127</v>
+      </c>
+      <c r="C58" t="s">
+        <v>128</v>
+      </c>
+      <c r="D58" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="67" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C67" t="s">
         <v>3</v>
       </c>
-      <c r="D52" t="s">
+      <c r="D67" t="s">
         <v>4</v>
       </c>
-      <c r="E52" s="8" t="s">
+      <c r="E67" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="F52" t="s">
+      <c r="F67" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="53" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C53" t="s">
+    <row r="68" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C68" t="s">
         <v>3</v>
       </c>
-      <c r="D53" t="s">
+      <c r="D68" t="s">
         <v>5</v>
       </c>
-      <c r="E53" s="8" t="s">
+      <c r="E68" s="8" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="54" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C54" t="s">
+    <row r="69" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C69" t="s">
         <v>3</v>
       </c>
-      <c r="D54" t="s">
+      <c r="D69" t="s">
         <v>6</v>
       </c>
-      <c r="E54" s="8" t="s">
+      <c r="E69" s="8" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="56" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C56" t="s">
+    <row r="71" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C71" t="s">
         <v>13</v>
       </c>
-      <c r="D56" t="s">
+      <c r="D71" t="s">
         <v>14</v>
       </c>
-      <c r="E56" s="8" t="s">
+      <c r="E71" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="F56" t="s">
+      <c r="F71" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="60" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C60" t="s">
+    <row r="75" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C75" t="s">
         <v>16</v>
       </c>
-      <c r="E60" s="8" t="s">
+      <c r="E75" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="F60" t="s">
+      <c r="F75" t="s">
         <v>21</v>
       </c>
     </row>

</xml_diff>

<commit_message>
test case numbering cleared in xls
</commit_message>
<xml_diff>
--- a/car-count-test/car-count-test-cases.xlsx
+++ b/car-count-test/car-count-test-cases.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="259" uniqueCount="196">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="253" uniqueCount="202">
   <si>
     <t>description</t>
   </si>
@@ -291,31 +291,16 @@
     <t>car-count test cases</t>
   </si>
   <si>
-    <t>vel001</t>
-  </si>
-  <si>
     <t>addTrackEntry</t>
   </si>
   <si>
-    <t>vel002</t>
-  </si>
-  <si>
     <t>assignBlobs</t>
   </si>
   <si>
-    <t>ass001</t>
-  </si>
-  <si>
     <t>updateTrackIntersect</t>
   </si>
   <si>
     <t>setLeavingRoiFlag</t>
-  </si>
-  <si>
-    <t>vel003</t>
-  </si>
-  <si>
-    <t>id001</t>
   </si>
   <si>
     <t>Track constructor</t>
@@ -342,9 +327,6 @@
     <t>keep velocity</t>
   </si>
   <si>
-    <t>upd001</t>
-  </si>
-  <si>
     <t>intersection</t>
   </si>
   <si>
@@ -358,12 +340,6 @@
 assign leftmost, if moving to left</t>
   </si>
   <si>
-    <t>upd002</t>
-  </si>
-  <si>
-    <t>upd003</t>
-  </si>
-  <si>
     <t>confidence in- / decrease</t>
   </si>
   <si>
@@ -377,9 +353,6 @@
     <t>compose track entry from previous element</t>
   </si>
   <si>
-    <t>upd004</t>
-  </si>
-  <si>
     <t>flag depends on direction and position of blob</t>
   </si>
   <si>
@@ -419,21 +392,12 @@
     <t>occ005</t>
   </si>
   <si>
-    <t>com001</t>
-  </si>
-  <si>
     <t>combineTracks</t>
   </si>
   <si>
-    <t>del001</t>
-  </si>
-  <si>
     <t>deleteMarkedTracks</t>
   </si>
   <si>
-    <t>del002</t>
-  </si>
-  <si>
     <t>same direction and intersection</t>
   </si>
   <si>
@@ -446,9 +410,6 @@
     <t>track changes direction</t>
   </si>
   <si>
-    <t>vel004</t>
-  </si>
-  <si>
     <t>assign if not occluded</t>
   </si>
   <si>
@@ -474,9 +435,6 @@
   </si>
   <si>
     <t>calcSubstitute</t>
-  </si>
-  <si>
-    <t>occ006</t>
   </si>
   <si>
     <t>adjustSubstPos</t>
@@ -508,30 +466,18 @@
     <t>mark for deletion, if conf drops below 0</t>
   </si>
   <si>
-    <t>upd005</t>
-  </si>
-  <si>
     <t>mark for deletion, if substitute outside roi</t>
   </si>
   <si>
     <t xml:space="preserve">delete tracks outside roi </t>
   </si>
   <si>
-    <t>occ008</t>
-  </si>
-  <si>
     <t>[Occlusion]</t>
   </si>
   <si>
     <t>refactor to base class UniqueID</t>
   </si>
   <si>
-    <t>[fcn-track]</t>
-  </si>
-  <si>
-    <t>del003</t>
-  </si>
-  <si>
     <t>deleteOcclusionWithMarkedTracks</t>
   </si>
   <si>
@@ -541,9 +487,6 @@
     <t>countVehicles</t>
   </si>
   <si>
-    <t>id002</t>
-  </si>
-  <si>
     <t>id</t>
   </si>
   <si>
@@ -553,24 +496,15 @@
     <t>change occlusion rect based on track rects</t>
   </si>
   <si>
-    <t>pas001</t>
-  </si>
-  <si>
     <t>hasPassed</t>
   </si>
   <si>
-    <t>con001</t>
-  </si>
-  <si>
     <t>constructor</t>
   </si>
   <si>
     <t>[OcclusionIdList]</t>
   </si>
   <si>
-    <t>add001</t>
-  </si>
-  <si>
     <t>addOcclusion</t>
   </si>
   <si>
@@ -583,24 +517,9 @@
     <t>remove</t>
   </si>
   <si>
-    <t>get001</t>
-  </si>
-  <si>
-    <t>rem001</t>
-  </si>
-  <si>
-    <t>returnTrackID</t>
-  </si>
-  <si>
-    <t>getTrackID</t>
-  </si>
-  <si>
     <t>occlusionList</t>
   </si>
   <si>
-    <t>obs001</t>
-  </si>
-  <si>
     <t>update</t>
   </si>
   <si>
@@ -614,6 +533,105 @@
   </si>
   <si>
     <t>setID</t>
+  </si>
+  <si>
+    <t>trk001</t>
+  </si>
+  <si>
+    <t>trk002</t>
+  </si>
+  <si>
+    <t>trk003</t>
+  </si>
+  <si>
+    <t>trk004</t>
+  </si>
+  <si>
+    <t>trk005</t>
+  </si>
+  <si>
+    <t>trk006</t>
+  </si>
+  <si>
+    <t>trk007</t>
+  </si>
+  <si>
+    <t>trk008</t>
+  </si>
+  <si>
+    <t>trk009</t>
+  </si>
+  <si>
+    <t>trk010</t>
+  </si>
+  <si>
+    <t>ocl001</t>
+  </si>
+  <si>
+    <t>ocl002</t>
+  </si>
+  <si>
+    <t>ocl003</t>
+  </si>
+  <si>
+    <t>ocl004</t>
+  </si>
+  <si>
+    <t>ocl005</t>
+  </si>
+  <si>
+    <t>ocl006</t>
+  </si>
+  <si>
+    <t>sce001</t>
+  </si>
+  <si>
+    <t>sce002</t>
+  </si>
+  <si>
+    <t>[fcn-scene]</t>
+  </si>
+  <si>
+    <t>sce003</t>
+  </si>
+  <si>
+    <t>sce004</t>
+  </si>
+  <si>
+    <t>sce005</t>
+  </si>
+  <si>
+    <t>sce006</t>
+  </si>
+  <si>
+    <t>sce007</t>
+  </si>
+  <si>
+    <t>sce008</t>
+  </si>
+  <si>
+    <t>sce009</t>
+  </si>
+  <si>
+    <t>sce010</t>
+  </si>
+  <si>
+    <t>sce011</t>
+  </si>
+  <si>
+    <t>sce012</t>
+  </si>
+  <si>
+    <t>getTrackID, returnTrackID</t>
+  </si>
+  <si>
+    <t>sce013</t>
+  </si>
+  <si>
+    <t>sce014</t>
+  </si>
+  <si>
+    <t>sce015</t>
   </si>
 </sst>
 </file>
@@ -1047,13 +1065,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G75"/>
+  <dimension ref="A1:G74"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="5" ySplit="2" topLeftCell="F17" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="5" ySplit="2" topLeftCell="F3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="C29" sqref="C29"/>
+      <selection pane="bottomRight" activeCell="C51" sqref="C51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1075,7 +1093,7 @@
         <v>68</v>
       </c>
       <c r="E1" s="19" t="s">
-        <v>194</v>
+        <v>167</v>
       </c>
       <c r="F1" s="20" t="s">
         <v>69</v>
@@ -1270,7 +1288,7 @@
         <v>85</v>
       </c>
       <c r="C14" s="8" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
     </row>
     <row r="16" spans="1:7" s="16" customFormat="1" x14ac:dyDescent="0.25">
@@ -1278,13 +1296,13 @@
         <v>87</v>
       </c>
       <c r="B16" s="15" t="s">
-        <v>99</v>
+        <v>169</v>
       </c>
       <c r="C16" s="16" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="D16" s="16" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="E16" s="17"/>
     </row>
@@ -1293,16 +1311,16 @@
         <v>87</v>
       </c>
       <c r="B17" s="5" t="s">
+        <v>170</v>
+      </c>
+      <c r="C17" t="s">
         <v>91</v>
       </c>
-      <c r="C17" t="s">
-        <v>92</v>
-      </c>
       <c r="D17" s="8" t="s">
-        <v>102</v>
+        <v>97</v>
       </c>
       <c r="E17" s="8" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
@@ -1310,16 +1328,16 @@
         <v>87</v>
       </c>
       <c r="B18" s="5" t="s">
-        <v>93</v>
+        <v>171</v>
       </c>
       <c r="C18" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D18" s="8" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
       <c r="E18" s="8" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
     </row>
     <row r="19" spans="1:5" ht="30" x14ac:dyDescent="0.25">
@@ -1327,16 +1345,16 @@
         <v>87</v>
       </c>
       <c r="B19" s="5" t="s">
-        <v>98</v>
+        <v>172</v>
       </c>
       <c r="C19" t="s">
-        <v>115</v>
+        <v>107</v>
       </c>
       <c r="D19" s="8" t="s">
-        <v>117</v>
+        <v>109</v>
       </c>
       <c r="E19" s="8" t="s">
-        <v>116</v>
+        <v>108</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
@@ -1344,16 +1362,16 @@
         <v>87</v>
       </c>
       <c r="B20" s="5" t="s">
-        <v>141</v>
+        <v>173</v>
       </c>
       <c r="C20" t="s">
-        <v>139</v>
+        <v>127</v>
       </c>
       <c r="D20" s="8" t="s">
-        <v>140</v>
+        <v>128</v>
       </c>
       <c r="E20" s="8" t="s">
-        <v>143</v>
+        <v>130</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
@@ -1361,16 +1379,16 @@
         <v>87</v>
       </c>
       <c r="B21" s="5" t="s">
-        <v>107</v>
+        <v>174</v>
       </c>
       <c r="C21" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="D21" s="8" t="s">
-        <v>108</v>
+        <v>102</v>
       </c>
       <c r="E21" s="8" t="s">
-        <v>109</v>
+        <v>103</v>
       </c>
     </row>
     <row r="22" spans="1:5" ht="30" x14ac:dyDescent="0.25">
@@ -1378,16 +1396,16 @@
         <v>87</v>
       </c>
       <c r="B22" s="5" t="s">
-        <v>112</v>
+        <v>175</v>
       </c>
       <c r="C22" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="D22" s="8" t="s">
-        <v>110</v>
+        <v>104</v>
       </c>
       <c r="E22" s="8" t="s">
-        <v>111</v>
+        <v>105</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
@@ -1395,16 +1413,16 @@
         <v>87</v>
       </c>
       <c r="B23" s="5" t="s">
-        <v>113</v>
+        <v>176</v>
       </c>
       <c r="C23" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="D23" s="8" t="s">
-        <v>114</v>
+        <v>106</v>
       </c>
       <c r="E23" s="8" t="s">
-        <v>159</v>
+        <v>145</v>
       </c>
     </row>
     <row r="24" spans="1:5" ht="30" x14ac:dyDescent="0.25">
@@ -1412,16 +1430,16 @@
         <v>87</v>
       </c>
       <c r="B24" s="5" t="s">
-        <v>118</v>
+        <v>177</v>
       </c>
       <c r="C24" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="D24" s="8" t="s">
-        <v>119</v>
+        <v>110</v>
       </c>
       <c r="E24" s="8" t="s">
-        <v>120</v>
+        <v>111</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
@@ -1429,16 +1447,16 @@
         <v>87</v>
       </c>
       <c r="B25" s="5" t="s">
-        <v>160</v>
+        <v>178</v>
       </c>
       <c r="C25" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="D25" s="8" t="s">
-        <v>162</v>
+        <v>147</v>
       </c>
       <c r="E25" s="8" t="s">
-        <v>161</v>
+        <v>146</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
@@ -1447,70 +1465,70 @@
     </row>
     <row r="27" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>164</v>
+        <v>148</v>
       </c>
       <c r="B27" s="12" t="s">
-        <v>95</v>
+        <v>118</v>
       </c>
       <c r="C27" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="D27" s="8" t="s">
-        <v>156</v>
+        <v>142</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>164</v>
+        <v>148</v>
       </c>
       <c r="B28" s="5" t="s">
-        <v>99</v>
+        <v>89</v>
       </c>
       <c r="C28" t="s">
-        <v>172</v>
+        <v>153</v>
       </c>
       <c r="D28" s="8"/>
       <c r="E28" s="11" t="s">
-        <v>165</v>
+        <v>149</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>164</v>
+        <v>148</v>
       </c>
       <c r="B29" s="5" t="s">
-        <v>171</v>
+        <v>117</v>
       </c>
       <c r="C29" t="s">
-        <v>195</v>
+        <v>168</v>
       </c>
       <c r="D29" s="8"/>
       <c r="E29" s="11"/>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>164</v>
+        <v>148</v>
       </c>
       <c r="B30" s="12" t="s">
-        <v>175</v>
+        <v>133</v>
       </c>
       <c r="C30" t="s">
-        <v>176</v>
+        <v>156</v>
       </c>
       <c r="D30" s="8"/>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>164</v>
+        <v>148</v>
       </c>
       <c r="B31" s="12" t="s">
-        <v>107</v>
+        <v>122</v>
       </c>
       <c r="C31" t="s">
-        <v>173</v>
+        <v>154</v>
       </c>
       <c r="D31" s="8" t="s">
-        <v>174</v>
+        <v>155</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
@@ -1519,134 +1537,135 @@
     </row>
     <row r="33" spans="1:5" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A33" s="16" t="s">
+        <v>158</v>
+      </c>
+      <c r="B33" s="18" t="s">
         <v>179</v>
       </c>
-      <c r="B33" s="18" t="s">
-        <v>177</v>
-      </c>
       <c r="C33" s="16" t="s">
-        <v>178</v>
+        <v>157</v>
       </c>
       <c r="D33" s="17"/>
       <c r="E33" s="17"/>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>179</v>
+        <v>158</v>
       </c>
       <c r="B34" s="12" t="s">
         <v>180</v>
       </c>
       <c r="C34" t="s">
-        <v>181</v>
+        <v>159</v>
       </c>
       <c r="D34" s="8"/>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>179</v>
+        <v>158</v>
       </c>
       <c r="B35" s="12" t="s">
-        <v>95</v>
+        <v>181</v>
       </c>
       <c r="C35" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="D35" s="8"/>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>179</v>
+        <v>158</v>
       </c>
       <c r="B36" s="12" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="C36" t="s">
-        <v>182</v>
+        <v>160</v>
       </c>
       <c r="D36" s="8"/>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>179</v>
+        <v>158</v>
       </c>
       <c r="B37" s="12" t="s">
-        <v>89</v>
+        <v>183</v>
       </c>
       <c r="C37" t="s">
-        <v>183</v>
+        <v>161</v>
       </c>
       <c r="D37" s="8"/>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>179</v>
+        <v>158</v>
       </c>
       <c r="B38" s="12" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="C38" t="s">
-        <v>184</v>
+        <v>162</v>
       </c>
       <c r="D38" s="8"/>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D39" s="8"/>
     </row>
-    <row r="40" spans="1:5" s="16" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="16" t="s">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
         <v>88</v>
       </c>
-      <c r="B40" s="18" t="s">
-        <v>177</v>
-      </c>
-      <c r="C40" s="16" t="s">
-        <v>178</v>
-      </c>
-      <c r="D40" s="17"/>
-      <c r="E40" s="17"/>
+      <c r="B40" s="13" t="s">
+        <v>186</v>
+      </c>
+      <c r="C40" t="s">
+        <v>92</v>
+      </c>
+      <c r="D40" s="8" t="s">
+        <v>129</v>
+      </c>
+      <c r="E40" s="8" t="s">
+        <v>112</v>
+      </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>88</v>
       </c>
-      <c r="B41" s="13" t="s">
-        <v>95</v>
+      <c r="B41" s="12" t="s">
+        <v>151</v>
       </c>
       <c r="C41" t="s">
-        <v>94</v>
-      </c>
-      <c r="D41" s="8" t="s">
-        <v>142</v>
-      </c>
-      <c r="E41" s="8" t="s">
-        <v>121</v>
-      </c>
+        <v>152</v>
+      </c>
+      <c r="D41" s="8"/>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>88</v>
       </c>
-      <c r="B42" s="12" t="s">
-        <v>169</v>
+      <c r="B42" s="5" t="s">
+        <v>189</v>
       </c>
       <c r="C42" t="s">
-        <v>170</v>
-      </c>
-      <c r="D42" s="8"/>
+        <v>124</v>
+      </c>
+      <c r="D42" s="8" t="s">
+        <v>126</v>
+      </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>88</v>
       </c>
       <c r="B43" s="5" t="s">
-        <v>134</v>
+        <v>190</v>
       </c>
       <c r="C43" t="s">
-        <v>135</v>
+        <v>150</v>
       </c>
       <c r="D43" s="8" t="s">
-        <v>138</v>
+        <v>166</v>
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.25">
@@ -1654,13 +1673,13 @@
         <v>88</v>
       </c>
       <c r="B44" s="5" t="s">
-        <v>167</v>
+        <v>191</v>
       </c>
       <c r="C44" t="s">
-        <v>168</v>
+        <v>132</v>
       </c>
       <c r="D44" s="8" t="s">
-        <v>193</v>
+        <v>126</v>
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.25">
@@ -1668,189 +1687,178 @@
         <v>88</v>
       </c>
       <c r="B45" s="5" t="s">
-        <v>136</v>
-      </c>
-      <c r="C45" t="s">
-        <v>145</v>
-      </c>
-      <c r="D45" s="8" t="s">
-        <v>138</v>
+        <v>185</v>
+      </c>
+      <c r="C45" s="8" t="s">
+        <v>198</v>
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>88</v>
       </c>
-      <c r="B46" s="5" t="s">
-        <v>99</v>
-      </c>
-      <c r="C46" s="8" t="s">
-        <v>188</v>
+      <c r="B46" s="12" t="s">
+        <v>199</v>
+      </c>
+      <c r="C46" t="s">
+        <v>163</v>
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>88</v>
       </c>
-      <c r="B47" s="12" t="s">
-        <v>163</v>
+      <c r="B47" s="5" t="s">
+        <v>195</v>
       </c>
       <c r="C47" t="s">
-        <v>189</v>
+        <v>136</v>
+      </c>
+      <c r="D47" t="s">
+        <v>134</v>
+      </c>
+      <c r="E47" s="8" t="s">
+        <v>135</v>
       </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>88</v>
       </c>
-      <c r="B48" s="5" t="s">
-        <v>171</v>
+      <c r="B48" s="12" t="s">
+        <v>200</v>
       </c>
       <c r="C48" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
+        <v>164</v>
+      </c>
+      <c r="D48" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" ht="75" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>88</v>
       </c>
-      <c r="B49" s="5" t="s">
-        <v>146</v>
+      <c r="B49" s="13" t="s">
+        <v>201</v>
       </c>
       <c r="C49" t="s">
-        <v>149</v>
+        <v>141</v>
       </c>
       <c r="D49" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="E49" s="8" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A50" t="s">
-        <v>88</v>
-      </c>
-      <c r="B50" s="5" t="s">
-        <v>190</v>
-      </c>
-      <c r="C50" t="s">
-        <v>191</v>
-      </c>
-      <c r="D50" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="51" spans="1:5" ht="75" x14ac:dyDescent="0.25">
-      <c r="A51" t="s">
-        <v>88</v>
-      </c>
-      <c r="B51" s="5" t="s">
-        <v>107</v>
-      </c>
-      <c r="C51" t="s">
-        <v>155</v>
-      </c>
-      <c r="D51" t="s">
-        <v>157</v>
-      </c>
-      <c r="E51" s="8" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B52" s="10"/>
-      <c r="D52" s="8"/>
-    </row>
-    <row r="53" spans="1:5" s="16" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A53" s="16" t="s">
-        <v>166</v>
-      </c>
-      <c r="B53" s="15" t="s">
-        <v>151</v>
-      </c>
-      <c r="C53" s="16" t="s">
-        <v>152</v>
-      </c>
-      <c r="D53" s="16" t="s">
-        <v>153</v>
-      </c>
-      <c r="E53" s="17"/>
+        <v>144</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B51" s="10"/>
+      <c r="D51" s="8"/>
+    </row>
+    <row r="52" spans="1:5" s="16" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A52" s="16" t="s">
+        <v>187</v>
+      </c>
+      <c r="B52" s="15" t="s">
+        <v>197</v>
+      </c>
+      <c r="C52" s="16" t="s">
+        <v>138</v>
+      </c>
+      <c r="D52" s="16" t="s">
+        <v>139</v>
+      </c>
+      <c r="E52" s="17"/>
+    </row>
+    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
+        <v>187</v>
+      </c>
+      <c r="B53" s="5" t="s">
+        <v>196</v>
+      </c>
+      <c r="C53" t="s">
+        <v>137</v>
+      </c>
+      <c r="D53" t="s">
+        <v>140</v>
+      </c>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>166</v>
+        <v>187</v>
       </c>
       <c r="B54" s="5" t="s">
+        <v>188</v>
+      </c>
+      <c r="C54" t="s">
+        <v>123</v>
+      </c>
+      <c r="D54" s="8" t="s">
+        <v>125</v>
+      </c>
+      <c r="E54" s="8" t="s">
         <v>131</v>
-      </c>
-      <c r="C54" t="s">
-        <v>150</v>
-      </c>
-      <c r="D54" t="s">
-        <v>154</v>
       </c>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>166</v>
+        <v>187</v>
       </c>
       <c r="B55" s="5" t="s">
-        <v>132</v>
+        <v>192</v>
       </c>
       <c r="C55" t="s">
-        <v>133</v>
-      </c>
-      <c r="D55" s="8" t="s">
-        <v>137</v>
+        <v>113</v>
+      </c>
+      <c r="D55" t="s">
+        <v>114</v>
       </c>
       <c r="E55" s="8" t="s">
-        <v>144</v>
+        <v>115</v>
       </c>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>166</v>
+        <v>187</v>
       </c>
       <c r="B56" s="5" t="s">
-        <v>89</v>
+        <v>193</v>
       </c>
       <c r="C56" t="s">
-        <v>122</v>
+        <v>116</v>
       </c>
       <c r="D56" t="s">
-        <v>123</v>
-      </c>
-      <c r="E56" s="8" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>166</v>
+        <v>187</v>
       </c>
       <c r="B57" s="5" t="s">
-        <v>126</v>
+        <v>194</v>
       </c>
       <c r="C57" t="s">
-        <v>125</v>
+        <v>119</v>
       </c>
       <c r="D57" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A58" t="s">
-        <v>166</v>
-      </c>
-      <c r="B58" s="5" t="s">
-        <v>127</v>
-      </c>
-      <c r="C58" t="s">
-        <v>128</v>
-      </c>
-      <c r="D58" t="s">
-        <v>130</v>
+        <v>121</v>
+      </c>
+    </row>
+    <row r="66" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C66" t="s">
+        <v>3</v>
+      </c>
+      <c r="D66" t="s">
+        <v>4</v>
+      </c>
+      <c r="E66" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="F66" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="67" spans="3:6" x14ac:dyDescent="0.25">
@@ -1858,13 +1866,10 @@
         <v>3</v>
       </c>
       <c r="D67" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="E67" s="8" t="s">
-        <v>8</v>
-      </c>
-      <c r="F67" t="s">
-        <v>19</v>
+        <v>9</v>
       </c>
     </row>
     <row r="68" spans="3:6" x14ac:dyDescent="0.25">
@@ -1872,45 +1877,34 @@
         <v>3</v>
       </c>
       <c r="D68" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="E68" s="8" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="69" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C69" t="s">
-        <v>3</v>
-      </c>
-      <c r="D69" t="s">
-        <v>6</v>
-      </c>
-      <c r="E69" s="8" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="71" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C71" t="s">
+    <row r="70" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C70" t="s">
         <v>13</v>
       </c>
-      <c r="D71" t="s">
+      <c r="D70" t="s">
         <v>14</v>
       </c>
-      <c r="E71" s="8" t="s">
+      <c r="E70" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="F71" t="s">
+      <c r="F70" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="75" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C75" t="s">
+    <row r="74" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C74" t="s">
         <v>16</v>
       </c>
-      <c r="E75" s="8" t="s">
+      <c r="E74" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="F75" t="s">
+      <c r="F74" t="s">
         <v>21</v>
       </c>
     </row>

</xml_diff>

<commit_message>
test cases occlusion finished
</commit_message>
<xml_diff>
--- a/car-count-test/car-count-test-cases.xlsx
+++ b/car-count-test/car-count-test-cases.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="253" uniqueCount="202">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="246" uniqueCount="199">
   <si>
     <t>description</t>
   </si>
@@ -475,15 +475,9 @@
     <t>[Occlusion]</t>
   </si>
   <si>
-    <t>refactor to base class UniqueID</t>
-  </si>
-  <si>
     <t>deleteOcclusionWithMarkedTracks</t>
   </si>
   <si>
-    <t>cnt001</t>
-  </si>
-  <si>
     <t>countVehicles</t>
   </si>
   <si>
@@ -499,24 +493,9 @@
     <t>hasPassed</t>
   </si>
   <si>
-    <t>constructor</t>
-  </si>
-  <si>
     <t>[OcclusionIdList]</t>
   </si>
   <si>
-    <t>addOcclusion</t>
-  </si>
-  <si>
-    <t>getList</t>
-  </si>
-  <si>
-    <t>isOcclusion</t>
-  </si>
-  <si>
-    <t>remove</t>
-  </si>
-  <si>
     <t>occlusionList</t>
   </si>
   <si>
@@ -571,18 +550,6 @@
     <t>ocl002</t>
   </si>
   <si>
-    <t>ocl003</t>
-  </si>
-  <si>
-    <t>ocl004</t>
-  </si>
-  <si>
-    <t>ocl005</t>
-  </si>
-  <si>
-    <t>ocl006</t>
-  </si>
-  <si>
     <t>sce001</t>
   </si>
   <si>
@@ -632,6 +599,30 @@
   </si>
   <si>
     <t>sce015</t>
+  </si>
+  <si>
+    <t xml:space="preserve">construct with id (default=0) </t>
+  </si>
+  <si>
+    <t>set specified id</t>
+  </si>
+  <si>
+    <t>flag if occlusion has passed</t>
+  </si>
+  <si>
+    <t>add, remove</t>
+  </si>
+  <si>
+    <t>add, remove occclusion, getList</t>
+  </si>
+  <si>
+    <t>isOcclusion -&gt; true / false</t>
+  </si>
+  <si>
+    <t>assign blobs for all occlusions</t>
+  </si>
+  <si>
+    <t>sce016</t>
   </si>
 </sst>
 </file>
@@ -723,7 +714,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -752,7 +743,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -1065,13 +1055,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G74"/>
+  <dimension ref="A1:G70"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="5" ySplit="2" topLeftCell="F3" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="5" ySplit="2" topLeftCell="F17" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="C51" sqref="C51"/>
+      <selection pane="bottomRight" activeCell="B36" sqref="B36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1092,10 +1082,10 @@
       <c r="D1" s="9" t="s">
         <v>68</v>
       </c>
-      <c r="E1" s="19" t="s">
-        <v>167</v>
-      </c>
-      <c r="F1" s="20" t="s">
+      <c r="E1" s="18" t="s">
+        <v>160</v>
+      </c>
+      <c r="F1" s="19" t="s">
         <v>69</v>
       </c>
     </row>
@@ -1296,7 +1286,7 @@
         <v>87</v>
       </c>
       <c r="B16" s="15" t="s">
-        <v>169</v>
+        <v>162</v>
       </c>
       <c r="C16" s="16" t="s">
         <v>95</v>
@@ -1311,7 +1301,7 @@
         <v>87</v>
       </c>
       <c r="B17" s="5" t="s">
-        <v>170</v>
+        <v>163</v>
       </c>
       <c r="C17" t="s">
         <v>91</v>
@@ -1328,7 +1318,7 @@
         <v>87</v>
       </c>
       <c r="B18" s="5" t="s">
-        <v>171</v>
+        <v>164</v>
       </c>
       <c r="C18" t="s">
         <v>91</v>
@@ -1345,7 +1335,7 @@
         <v>87</v>
       </c>
       <c r="B19" s="5" t="s">
-        <v>172</v>
+        <v>165</v>
       </c>
       <c r="C19" t="s">
         <v>107</v>
@@ -1362,7 +1352,7 @@
         <v>87</v>
       </c>
       <c r="B20" s="5" t="s">
-        <v>173</v>
+        <v>166</v>
       </c>
       <c r="C20" t="s">
         <v>127</v>
@@ -1379,7 +1369,7 @@
         <v>87</v>
       </c>
       <c r="B21" s="5" t="s">
-        <v>174</v>
+        <v>167</v>
       </c>
       <c r="C21" t="s">
         <v>93</v>
@@ -1396,7 +1386,7 @@
         <v>87</v>
       </c>
       <c r="B22" s="5" t="s">
-        <v>175</v>
+        <v>168</v>
       </c>
       <c r="C22" t="s">
         <v>93</v>
@@ -1413,7 +1403,7 @@
         <v>87</v>
       </c>
       <c r="B23" s="5" t="s">
-        <v>176</v>
+        <v>169</v>
       </c>
       <c r="C23" t="s">
         <v>93</v>
@@ -1430,7 +1420,7 @@
         <v>87</v>
       </c>
       <c r="B24" s="5" t="s">
-        <v>177</v>
+        <v>170</v>
       </c>
       <c r="C24" t="s">
         <v>94</v>
@@ -1447,7 +1437,7 @@
         <v>87</v>
       </c>
       <c r="B25" s="5" t="s">
-        <v>178</v>
+        <v>171</v>
       </c>
       <c r="C25" t="s">
         <v>93</v>
@@ -1467,7 +1457,7 @@
       <c r="A27" t="s">
         <v>148</v>
       </c>
-      <c r="B27" s="12" t="s">
+      <c r="B27" s="5" t="s">
         <v>118</v>
       </c>
       <c r="C27" t="s">
@@ -1485,12 +1475,12 @@
         <v>89</v>
       </c>
       <c r="C28" t="s">
-        <v>153</v>
-      </c>
-      <c r="D28" s="8"/>
-      <c r="E28" s="11" t="s">
-        <v>149</v>
-      </c>
+        <v>151</v>
+      </c>
+      <c r="D28" s="8" t="s">
+        <v>191</v>
+      </c>
+      <c r="E28" s="11"/>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
@@ -1500,35 +1490,39 @@
         <v>117</v>
       </c>
       <c r="C29" t="s">
-        <v>168</v>
-      </c>
-      <c r="D29" s="8"/>
+        <v>161</v>
+      </c>
+      <c r="D29" s="8" t="s">
+        <v>192</v>
+      </c>
       <c r="E29" s="11"/>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>148</v>
       </c>
-      <c r="B30" s="12" t="s">
+      <c r="B30" s="5" t="s">
         <v>133</v>
       </c>
       <c r="C30" t="s">
-        <v>156</v>
-      </c>
-      <c r="D30" s="8"/>
+        <v>154</v>
+      </c>
+      <c r="D30" s="8" t="s">
+        <v>193</v>
+      </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>148</v>
       </c>
-      <c r="B31" s="12" t="s">
+      <c r="B31" s="5" t="s">
         <v>122</v>
       </c>
       <c r="C31" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="D31" s="8" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
@@ -1537,121 +1531,129 @@
     </row>
     <row r="33" spans="1:5" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A33" s="16" t="s">
-        <v>158</v>
-      </c>
-      <c r="B33" s="18" t="s">
-        <v>179</v>
+        <v>155</v>
+      </c>
+      <c r="B33" s="15" t="s">
+        <v>172</v>
       </c>
       <c r="C33" s="16" t="s">
-        <v>157</v>
-      </c>
-      <c r="D33" s="17"/>
-      <c r="E33" s="17"/>
+        <v>194</v>
+      </c>
+      <c r="D33" s="17" t="s">
+        <v>195</v>
+      </c>
+      <c r="E33" s="17" t="s">
+        <v>196</v>
+      </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>158</v>
-      </c>
-      <c r="B34" s="12" t="s">
-        <v>180</v>
+        <v>155</v>
+      </c>
+      <c r="B34" s="5" t="s">
+        <v>173</v>
       </c>
       <c r="C34" t="s">
-        <v>159</v>
-      </c>
-      <c r="D34" s="8"/>
+        <v>92</v>
+      </c>
+      <c r="D34" s="8" t="s">
+        <v>197</v>
+      </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A35" t="s">
-        <v>158</v>
-      </c>
-      <c r="B35" s="12" t="s">
-        <v>181</v>
-      </c>
-      <c r="C35" t="s">
+      <c r="D35" s="8"/>
+    </row>
+    <row r="36" spans="1:5" s="16" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A36" s="16" t="s">
+        <v>88</v>
+      </c>
+      <c r="B36" s="15" t="s">
+        <v>175</v>
+      </c>
+      <c r="C36" s="16" t="s">
         <v>92</v>
       </c>
-      <c r="D35" s="8"/>
-    </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A36" t="s">
-        <v>158</v>
-      </c>
-      <c r="B36" s="12" t="s">
-        <v>182</v>
-      </c>
-      <c r="C36" t="s">
-        <v>160</v>
-      </c>
-      <c r="D36" s="8"/>
+      <c r="D36" s="17" t="s">
+        <v>129</v>
+      </c>
+      <c r="E36" s="17" t="s">
+        <v>112</v>
+      </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>158</v>
+        <v>88</v>
       </c>
       <c r="B37" s="12" t="s">
-        <v>183</v>
+        <v>198</v>
       </c>
       <c r="C37" t="s">
-        <v>161</v>
+        <v>150</v>
       </c>
       <c r="D37" s="8"/>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>158</v>
-      </c>
-      <c r="B38" s="12" t="s">
-        <v>184</v>
+        <v>88</v>
+      </c>
+      <c r="B38" s="5" t="s">
+        <v>178</v>
       </c>
       <c r="C38" t="s">
-        <v>162</v>
-      </c>
-      <c r="D38" s="8"/>
+        <v>124</v>
+      </c>
+      <c r="D38" s="8" t="s">
+        <v>126</v>
+      </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="D39" s="8"/>
+      <c r="A39" t="s">
+        <v>88</v>
+      </c>
+      <c r="B39" s="5" t="s">
+        <v>179</v>
+      </c>
+      <c r="C39" t="s">
+        <v>149</v>
+      </c>
+      <c r="D39" s="8" t="s">
+        <v>159</v>
+      </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>88</v>
       </c>
-      <c r="B40" s="13" t="s">
-        <v>186</v>
+      <c r="B40" s="5" t="s">
+        <v>180</v>
       </c>
       <c r="C40" t="s">
-        <v>92</v>
+        <v>132</v>
       </c>
       <c r="D40" s="8" t="s">
-        <v>129</v>
-      </c>
-      <c r="E40" s="8" t="s">
-        <v>112</v>
+        <v>126</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>88</v>
       </c>
-      <c r="B41" s="12" t="s">
-        <v>151</v>
-      </c>
-      <c r="C41" t="s">
-        <v>152</v>
-      </c>
-      <c r="D41" s="8"/>
+      <c r="B41" s="5" t="s">
+        <v>174</v>
+      </c>
+      <c r="C41" s="8" t="s">
+        <v>187</v>
+      </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>88</v>
       </c>
-      <c r="B42" s="5" t="s">
-        <v>189</v>
+      <c r="B42" s="12" t="s">
+        <v>188</v>
       </c>
       <c r="C42" t="s">
-        <v>124</v>
-      </c>
-      <c r="D42" s="8" t="s">
-        <v>126</v>
+        <v>156</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.25">
@@ -1659,252 +1661,202 @@
         <v>88</v>
       </c>
       <c r="B43" s="5" t="s">
-        <v>190</v>
+        <v>184</v>
       </c>
       <c r="C43" t="s">
-        <v>150</v>
-      </c>
-      <c r="D43" s="8" t="s">
-        <v>166</v>
+        <v>136</v>
+      </c>
+      <c r="D43" t="s">
+        <v>134</v>
+      </c>
+      <c r="E43" s="8" t="s">
+        <v>135</v>
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>88</v>
       </c>
-      <c r="B44" s="5" t="s">
-        <v>191</v>
+      <c r="B44" s="12" t="s">
+        <v>189</v>
       </c>
       <c r="C44" t="s">
-        <v>132</v>
-      </c>
-      <c r="D44" s="8" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
+        <v>157</v>
+      </c>
+      <c r="D44" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" ht="75" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>88</v>
       </c>
-      <c r="B45" s="5" t="s">
+      <c r="B45" s="13" t="s">
+        <v>190</v>
+      </c>
+      <c r="C45" t="s">
+        <v>141</v>
+      </c>
+      <c r="D45" t="s">
+        <v>143</v>
+      </c>
+      <c r="E45" s="8" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B47" s="10"/>
+      <c r="D47" s="8"/>
+    </row>
+    <row r="48" spans="1:5" s="16" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A48" s="16" t="s">
+        <v>176</v>
+      </c>
+      <c r="B48" s="15" t="s">
+        <v>186</v>
+      </c>
+      <c r="C48" s="16" t="s">
+        <v>138</v>
+      </c>
+      <c r="D48" s="16" t="s">
+        <v>139</v>
+      </c>
+      <c r="E48" s="17"/>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
+        <v>176</v>
+      </c>
+      <c r="B49" s="5" t="s">
         <v>185</v>
       </c>
-      <c r="C45" s="8" t="s">
-        <v>198</v>
-      </c>
-    </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A46" t="s">
-        <v>88</v>
-      </c>
-      <c r="B46" s="12" t="s">
-        <v>199</v>
-      </c>
-      <c r="C46" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A47" t="s">
-        <v>88</v>
-      </c>
-      <c r="B47" s="5" t="s">
-        <v>195</v>
-      </c>
-      <c r="C47" t="s">
-        <v>136</v>
-      </c>
-      <c r="D47" t="s">
-        <v>134</v>
-      </c>
-      <c r="E47" s="8" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A48" t="s">
-        <v>88</v>
-      </c>
-      <c r="B48" s="12" t="s">
-        <v>200</v>
-      </c>
-      <c r="C48" t="s">
-        <v>164</v>
-      </c>
-      <c r="D48" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="49" spans="1:5" ht="75" x14ac:dyDescent="0.25">
-      <c r="A49" t="s">
-        <v>88</v>
-      </c>
-      <c r="B49" s="13" t="s">
-        <v>201</v>
-      </c>
       <c r="C49" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
       <c r="D49" t="s">
-        <v>143</v>
-      </c>
-      <c r="E49" s="8" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B51" s="10"/>
-      <c r="D51" s="8"/>
-    </row>
-    <row r="52" spans="1:5" s="16" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A52" s="16" t="s">
-        <v>187</v>
-      </c>
-      <c r="B52" s="15" t="s">
-        <v>197</v>
-      </c>
-      <c r="C52" s="16" t="s">
-        <v>138</v>
-      </c>
-      <c r="D52" s="16" t="s">
-        <v>139</v>
-      </c>
-      <c r="E52" s="17"/>
-    </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>176</v>
+      </c>
+      <c r="B50" s="5" t="s">
+        <v>177</v>
+      </c>
+      <c r="C50" t="s">
+        <v>123</v>
+      </c>
+      <c r="D50" s="8" t="s">
+        <v>125</v>
+      </c>
+      <c r="E50" s="8" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>176</v>
+      </c>
+      <c r="B51" s="5" t="s">
+        <v>181</v>
+      </c>
+      <c r="C51" t="s">
+        <v>113</v>
+      </c>
+      <c r="D51" t="s">
+        <v>114</v>
+      </c>
+      <c r="E51" s="8" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
+        <v>176</v>
+      </c>
+      <c r="B52" s="5" t="s">
+        <v>182</v>
+      </c>
+      <c r="C52" t="s">
+        <v>116</v>
+      </c>
+      <c r="D52" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>187</v>
+        <v>176</v>
       </c>
       <c r="B53" s="5" t="s">
-        <v>196</v>
+        <v>183</v>
       </c>
       <c r="C53" t="s">
-        <v>137</v>
+        <v>119</v>
       </c>
       <c r="D53" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A54" t="s">
-        <v>187</v>
-      </c>
-      <c r="B54" s="5" t="s">
-        <v>188</v>
-      </c>
-      <c r="C54" t="s">
-        <v>123</v>
-      </c>
-      <c r="D54" s="8" t="s">
-        <v>125</v>
-      </c>
-      <c r="E54" s="8" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A55" t="s">
-        <v>187</v>
-      </c>
-      <c r="B55" s="5" t="s">
-        <v>192</v>
-      </c>
-      <c r="C55" t="s">
-        <v>113</v>
-      </c>
-      <c r="D55" t="s">
-        <v>114</v>
-      </c>
-      <c r="E55" s="8" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A56" t="s">
-        <v>187</v>
-      </c>
-      <c r="B56" s="5" t="s">
-        <v>193</v>
-      </c>
-      <c r="C56" t="s">
-        <v>116</v>
-      </c>
-      <c r="D56" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A57" t="s">
-        <v>187</v>
-      </c>
-      <c r="B57" s="5" t="s">
-        <v>194</v>
-      </c>
-      <c r="C57" t="s">
-        <v>119</v>
-      </c>
-      <c r="D57" t="s">
         <v>121</v>
+      </c>
+    </row>
+    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C62" t="s">
+        <v>3</v>
+      </c>
+      <c r="D62" t="s">
+        <v>4</v>
+      </c>
+      <c r="E62" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="F62" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C63" t="s">
+        <v>3</v>
+      </c>
+      <c r="D63" t="s">
+        <v>5</v>
+      </c>
+      <c r="E63" s="8" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C64" t="s">
+        <v>3</v>
+      </c>
+      <c r="D64" t="s">
+        <v>6</v>
+      </c>
+      <c r="E64" s="8" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="66" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C66" t="s">
-        <v>3</v>
+        <v>13</v>
       </c>
       <c r="D66" t="s">
-        <v>4</v>
+        <v>14</v>
       </c>
       <c r="E66" s="8" t="s">
-        <v>8</v>
+        <v>15</v>
       </c>
       <c r="F66" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="67" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C67" t="s">
-        <v>3</v>
-      </c>
-      <c r="D67" t="s">
-        <v>5</v>
-      </c>
-      <c r="E67" s="8" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="68" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C68" t="s">
-        <v>3</v>
-      </c>
-      <c r="D68" t="s">
-        <v>6</v>
-      </c>
-      <c r="E68" s="8" t="s">
-        <v>10</v>
+        <v>20</v>
       </c>
     </row>
     <row r="70" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C70" t="s">
-        <v>13</v>
-      </c>
-      <c r="D70" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="E70" s="8" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="F70" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="74" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C74" t="s">
-        <v>16</v>
-      </c>
-      <c r="E74" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="F74" t="s">
         <v>21</v>
       </c>
     </row>

</xml_diff>

<commit_message>
test cases [Scene] finished
</commit_message>
<xml_diff>
--- a/car-count-test/car-count-test-cases.xlsx
+++ b/car-count-test/car-count-test-cases.xlsx
@@ -453,9 +453,6 @@
 two blobs -&gt; regular assign</t>
   </si>
   <si>
-    <t>full assignment</t>
-  </si>
-  <si>
     <t>two blobs moving opposite:
 outside occlusion: assignBlobs
 create occlusion
@@ -623,6 +620,9 @@
   </si>
   <si>
     <t>sce016</t>
+  </si>
+  <si>
+    <t>focus on assignment outside occlusion</t>
   </si>
 </sst>
 </file>
@@ -714,7 +714,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -736,7 +736,6 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -1058,10 +1057,10 @@
   <dimension ref="A1:G70"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="5" ySplit="2" topLeftCell="F17" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="5" ySplit="2" topLeftCell="H15" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="B36" sqref="B36"/>
+      <selection pane="bottomRight" activeCell="D43" sqref="D43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1082,10 +1081,10 @@
       <c r="D1" s="9" t="s">
         <v>68</v>
       </c>
-      <c r="E1" s="18" t="s">
-        <v>160</v>
-      </c>
-      <c r="F1" s="19" t="s">
+      <c r="E1" s="17" t="s">
+        <v>159</v>
+      </c>
+      <c r="F1" s="18" t="s">
         <v>69</v>
       </c>
     </row>
@@ -1233,15 +1232,15 @@
       <c r="A10" s="3"/>
       <c r="B10" s="10"/>
     </row>
-    <row r="11" spans="1:7" s="16" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="14" t="s">
+    <row r="11" spans="1:7" s="15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="13" t="s">
         <v>82</v>
       </c>
-      <c r="B11" s="15" t="s">
+      <c r="B11" s="14" t="s">
         <v>78</v>
       </c>
-      <c r="E11" s="17"/>
-      <c r="F11" s="16" t="s">
+      <c r="E11" s="16"/>
+      <c r="F11" s="15" t="s">
         <v>74</v>
       </c>
     </row>
@@ -1281,27 +1280,27 @@
         <v>98</v>
       </c>
     </row>
-    <row r="16" spans="1:7" s="16" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="16" t="s">
+    <row r="16" spans="1:7" s="15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="15" t="s">
         <v>87</v>
       </c>
-      <c r="B16" s="15" t="s">
-        <v>162</v>
-      </c>
-      <c r="C16" s="16" t="s">
+      <c r="B16" s="14" t="s">
+        <v>161</v>
+      </c>
+      <c r="C16" s="15" t="s">
         <v>95</v>
       </c>
-      <c r="D16" s="16" t="s">
+      <c r="D16" s="15" t="s">
         <v>96</v>
       </c>
-      <c r="E16" s="17"/>
+      <c r="E16" s="16"/>
     </row>
     <row r="17" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>87</v>
       </c>
       <c r="B17" s="5" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="C17" t="s">
         <v>91</v>
@@ -1318,7 +1317,7 @@
         <v>87</v>
       </c>
       <c r="B18" s="5" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="C18" t="s">
         <v>91</v>
@@ -1335,7 +1334,7 @@
         <v>87</v>
       </c>
       <c r="B19" s="5" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="C19" t="s">
         <v>107</v>
@@ -1352,7 +1351,7 @@
         <v>87</v>
       </c>
       <c r="B20" s="5" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="C20" t="s">
         <v>127</v>
@@ -1369,7 +1368,7 @@
         <v>87</v>
       </c>
       <c r="B21" s="5" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="C21" t="s">
         <v>93</v>
@@ -1386,7 +1385,7 @@
         <v>87</v>
       </c>
       <c r="B22" s="5" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="C22" t="s">
         <v>93</v>
@@ -1403,7 +1402,7 @@
         <v>87</v>
       </c>
       <c r="B23" s="5" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="C23" t="s">
         <v>93</v>
@@ -1412,7 +1411,7 @@
         <v>106</v>
       </c>
       <c r="E23" s="8" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="24" spans="1:5" ht="30" x14ac:dyDescent="0.25">
@@ -1420,7 +1419,7 @@
         <v>87</v>
       </c>
       <c r="B24" s="5" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="C24" t="s">
         <v>94</v>
@@ -1437,16 +1436,16 @@
         <v>87</v>
       </c>
       <c r="B25" s="5" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="C25" t="s">
         <v>93</v>
       </c>
       <c r="D25" s="8" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="E25" s="8" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
@@ -1455,7 +1454,7 @@
     </row>
     <row r="27" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="B27" s="5" t="s">
         <v>118</v>
@@ -1469,114 +1468,114 @@
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="B28" s="5" t="s">
         <v>89</v>
       </c>
       <c r="C28" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="D28" s="8" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="E28" s="11"/>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="B29" s="5" t="s">
         <v>117</v>
       </c>
       <c r="C29" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="D29" s="8" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="E29" s="11"/>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="B30" s="5" t="s">
         <v>133</v>
       </c>
       <c r="C30" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="D30" s="8" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="B31" s="5" t="s">
         <v>122</v>
       </c>
       <c r="C31" t="s">
+        <v>151</v>
+      </c>
+      <c r="D31" s="8" t="s">
         <v>152</v>
-      </c>
-      <c r="D31" s="8" t="s">
-        <v>153</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B32" s="10"/>
       <c r="D32" s="8"/>
     </row>
-    <row r="33" spans="1:5" s="16" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="16" t="s">
-        <v>155</v>
-      </c>
-      <c r="B33" s="15" t="s">
-        <v>172</v>
-      </c>
-      <c r="C33" s="16" t="s">
+    <row r="33" spans="1:5" s="15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="15" t="s">
+        <v>154</v>
+      </c>
+      <c r="B33" s="14" t="s">
+        <v>171</v>
+      </c>
+      <c r="C33" s="15" t="s">
+        <v>193</v>
+      </c>
+      <c r="D33" s="16" t="s">
         <v>194</v>
       </c>
-      <c r="D33" s="17" t="s">
+      <c r="E33" s="16" t="s">
         <v>195</v>
-      </c>
-      <c r="E33" s="17" t="s">
-        <v>196</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B34" s="5" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="C34" t="s">
         <v>92</v>
       </c>
       <c r="D34" s="8" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D35" s="8"/>
     </row>
-    <row r="36" spans="1:5" s="16" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="16" t="s">
+    <row r="36" spans="1:5" s="15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A36" s="15" t="s">
         <v>88</v>
       </c>
-      <c r="B36" s="15" t="s">
-        <v>175</v>
-      </c>
-      <c r="C36" s="16" t="s">
+      <c r="B36" s="14" t="s">
+        <v>174</v>
+      </c>
+      <c r="C36" s="15" t="s">
         <v>92</v>
       </c>
-      <c r="D36" s="17" t="s">
+      <c r="D36" s="16" t="s">
         <v>129</v>
       </c>
-      <c r="E36" s="17" t="s">
+      <c r="E36" s="16" t="s">
         <v>112</v>
       </c>
     </row>
@@ -1585,10 +1584,10 @@
         <v>88</v>
       </c>
       <c r="B37" s="12" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="C37" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="D37" s="8"/>
     </row>
@@ -1597,7 +1596,7 @@
         <v>88</v>
       </c>
       <c r="B38" s="5" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="C38" t="s">
         <v>124</v>
@@ -1611,13 +1610,13 @@
         <v>88</v>
       </c>
       <c r="B39" s="5" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="C39" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="D39" s="8" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.25">
@@ -1625,7 +1624,7 @@
         <v>88</v>
       </c>
       <c r="B40" s="5" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="C40" t="s">
         <v>132</v>
@@ -1639,10 +1638,10 @@
         <v>88</v>
       </c>
       <c r="B41" s="5" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="C41" s="8" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.25">
@@ -1650,10 +1649,10 @@
         <v>88</v>
       </c>
       <c r="B42" s="12" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="C42" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.25">
@@ -1661,7 +1660,7 @@
         <v>88</v>
       </c>
       <c r="B43" s="5" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="C43" t="s">
         <v>136</v>
@@ -1678,57 +1677,57 @@
         <v>88</v>
       </c>
       <c r="B44" s="12" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="C44" t="s">
+        <v>156</v>
+      </c>
+      <c r="D44" t="s">
         <v>157</v>
-      </c>
-      <c r="D44" t="s">
-        <v>158</v>
       </c>
     </row>
     <row r="45" spans="1:5" ht="75" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>88</v>
       </c>
-      <c r="B45" s="13" t="s">
-        <v>190</v>
+      <c r="B45" s="5" t="s">
+        <v>189</v>
       </c>
       <c r="C45" t="s">
         <v>141</v>
       </c>
       <c r="D45" t="s">
+        <v>198</v>
+      </c>
+      <c r="E45" s="8" t="s">
         <v>143</v>
-      </c>
-      <c r="E45" s="8" t="s">
-        <v>144</v>
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B47" s="10"/>
       <c r="D47" s="8"/>
     </row>
-    <row r="48" spans="1:5" s="16" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A48" s="16" t="s">
-        <v>176</v>
-      </c>
-      <c r="B48" s="15" t="s">
-        <v>186</v>
-      </c>
-      <c r="C48" s="16" t="s">
+    <row r="48" spans="1:5" s="15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A48" s="15" t="s">
+        <v>175</v>
+      </c>
+      <c r="B48" s="14" t="s">
+        <v>185</v>
+      </c>
+      <c r="C48" s="15" t="s">
         <v>138</v>
       </c>
-      <c r="D48" s="16" t="s">
+      <c r="D48" s="15" t="s">
         <v>139</v>
       </c>
-      <c r="E48" s="17"/>
+      <c r="E48" s="16"/>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="B49" s="5" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="C49" t="s">
         <v>137</v>
@@ -1739,10 +1738,10 @@
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
+        <v>175</v>
+      </c>
+      <c r="B50" s="5" t="s">
         <v>176</v>
-      </c>
-      <c r="B50" s="5" t="s">
-        <v>177</v>
       </c>
       <c r="C50" t="s">
         <v>123</v>
@@ -1756,10 +1755,10 @@
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="B51" s="5" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="C51" t="s">
         <v>113</v>
@@ -1773,10 +1772,10 @@
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="B52" s="5" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="C52" t="s">
         <v>116</v>
@@ -1787,10 +1786,10 @@
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="B53" s="5" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="C53" t="s">
         <v>119</v>

</xml_diff>

<commit_message>
refactor utilities, inc and src introduced
</commit_message>
<xml_diff>
--- a/car-count-test/car-count-test-cases.xlsx
+++ b/car-count-test/car-count-test-cases.xlsx
@@ -446,9 +446,6 @@
     <t>based on average velocity</t>
   </si>
   <si>
-    <t>updateTracksIntersect</t>
-  </si>
-  <si>
     <t>one blob -&gt; assign adjusted substitute to track
 two blobs -&gt; regular assign</t>
   </si>
@@ -623,6 +620,9 @@
   </si>
   <si>
     <t>focus on assignment outside occlusion</t>
+  </si>
+  <si>
+    <t>updateTracks</t>
   </si>
 </sst>
 </file>
@@ -1057,10 +1057,10 @@
   <dimension ref="A1:G70"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="5" ySplit="2" topLeftCell="H15" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="5" ySplit="2" topLeftCell="H27" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="D43" sqref="D43"/>
+      <selection pane="bottomRight" activeCell="C45" sqref="C45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1082,7 +1082,7 @@
         <v>68</v>
       </c>
       <c r="E1" s="17" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="F1" s="18" t="s">
         <v>69</v>
@@ -1285,7 +1285,7 @@
         <v>87</v>
       </c>
       <c r="B16" s="14" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="C16" s="15" t="s">
         <v>95</v>
@@ -1300,7 +1300,7 @@
         <v>87</v>
       </c>
       <c r="B17" s="5" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="C17" t="s">
         <v>91</v>
@@ -1317,7 +1317,7 @@
         <v>87</v>
       </c>
       <c r="B18" s="5" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="C18" t="s">
         <v>91</v>
@@ -1334,7 +1334,7 @@
         <v>87</v>
       </c>
       <c r="B19" s="5" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="C19" t="s">
         <v>107</v>
@@ -1351,7 +1351,7 @@
         <v>87</v>
       </c>
       <c r="B20" s="5" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="C20" t="s">
         <v>127</v>
@@ -1368,7 +1368,7 @@
         <v>87</v>
       </c>
       <c r="B21" s="5" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="C21" t="s">
         <v>93</v>
@@ -1385,7 +1385,7 @@
         <v>87</v>
       </c>
       <c r="B22" s="5" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="C22" t="s">
         <v>93</v>
@@ -1402,7 +1402,7 @@
         <v>87</v>
       </c>
       <c r="B23" s="5" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="C23" t="s">
         <v>93</v>
@@ -1411,7 +1411,7 @@
         <v>106</v>
       </c>
       <c r="E23" s="8" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="24" spans="1:5" ht="30" x14ac:dyDescent="0.25">
@@ -1419,7 +1419,7 @@
         <v>87</v>
       </c>
       <c r="B24" s="5" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="C24" t="s">
         <v>94</v>
@@ -1436,16 +1436,16 @@
         <v>87</v>
       </c>
       <c r="B25" s="5" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="C25" t="s">
         <v>93</v>
       </c>
       <c r="D25" s="8" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="E25" s="8" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
@@ -1454,7 +1454,7 @@
     </row>
     <row r="27" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="B27" s="5" t="s">
         <v>118</v>
@@ -1463,65 +1463,65 @@
         <v>92</v>
       </c>
       <c r="D27" s="8" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="B28" s="5" t="s">
         <v>89</v>
       </c>
       <c r="C28" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="D28" s="8" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="E28" s="11"/>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="B29" s="5" t="s">
         <v>117</v>
       </c>
       <c r="C29" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="D29" s="8" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="E29" s="11"/>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="B30" s="5" t="s">
         <v>133</v>
       </c>
       <c r="C30" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="D30" s="8" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="B31" s="5" t="s">
         <v>122</v>
       </c>
       <c r="C31" t="s">
+        <v>150</v>
+      </c>
+      <c r="D31" s="8" t="s">
         <v>151</v>
-      </c>
-      <c r="D31" s="8" t="s">
-        <v>152</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
@@ -1530,33 +1530,33 @@
     </row>
     <row r="33" spans="1:5" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A33" s="15" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B33" s="14" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="C33" s="15" t="s">
+        <v>192</v>
+      </c>
+      <c r="D33" s="16" t="s">
         <v>193</v>
       </c>
-      <c r="D33" s="16" t="s">
+      <c r="E33" s="16" t="s">
         <v>194</v>
-      </c>
-      <c r="E33" s="16" t="s">
-        <v>195</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B34" s="5" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="C34" t="s">
         <v>92</v>
       </c>
       <c r="D34" s="8" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.25">
@@ -1567,7 +1567,7 @@
         <v>88</v>
       </c>
       <c r="B36" s="14" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="C36" s="15" t="s">
         <v>92</v>
@@ -1584,10 +1584,10 @@
         <v>88</v>
       </c>
       <c r="B37" s="12" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="C37" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="D37" s="8"/>
     </row>
@@ -1596,7 +1596,7 @@
         <v>88</v>
       </c>
       <c r="B38" s="5" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="C38" t="s">
         <v>124</v>
@@ -1610,13 +1610,13 @@
         <v>88</v>
       </c>
       <c r="B39" s="5" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="C39" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="D39" s="8" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.25">
@@ -1624,7 +1624,7 @@
         <v>88</v>
       </c>
       <c r="B40" s="5" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="C40" t="s">
         <v>132</v>
@@ -1638,10 +1638,10 @@
         <v>88</v>
       </c>
       <c r="B41" s="5" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="C41" s="8" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.25">
@@ -1649,10 +1649,10 @@
         <v>88</v>
       </c>
       <c r="B42" s="12" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="C42" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.25">
@@ -1660,7 +1660,7 @@
         <v>88</v>
       </c>
       <c r="B43" s="5" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="C43" t="s">
         <v>136</v>
@@ -1677,13 +1677,13 @@
         <v>88</v>
       </c>
       <c r="B44" s="12" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="C44" t="s">
+        <v>155</v>
+      </c>
+      <c r="D44" t="s">
         <v>156</v>
-      </c>
-      <c r="D44" t="s">
-        <v>157</v>
       </c>
     </row>
     <row r="45" spans="1:5" ht="75" x14ac:dyDescent="0.25">
@@ -1691,16 +1691,16 @@
         <v>88</v>
       </c>
       <c r="B45" s="5" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="C45" t="s">
-        <v>141</v>
+        <v>198</v>
       </c>
       <c r="D45" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="E45" s="8" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.25">
@@ -1709,10 +1709,10 @@
     </row>
     <row r="48" spans="1:5" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A48" s="15" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="B48" s="14" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="C48" s="15" t="s">
         <v>138</v>
@@ -1724,10 +1724,10 @@
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="B49" s="5" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="C49" t="s">
         <v>137</v>
@@ -1738,10 +1738,10 @@
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
+        <v>174</v>
+      </c>
+      <c r="B50" s="5" t="s">
         <v>175</v>
-      </c>
-      <c r="B50" s="5" t="s">
-        <v>176</v>
       </c>
       <c r="C50" t="s">
         <v>123</v>
@@ -1755,10 +1755,10 @@
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="B51" s="5" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="C51" t="s">
         <v>113</v>
@@ -1772,10 +1772,10 @@
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="B52" s="5" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="C52" t="s">
         <v>116</v>
@@ -1786,10 +1786,10 @@
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="B53" s="5" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="C53" t="s">
         <v>119</v>

</xml_diff>

<commit_message>
fixed: #21 track extension at roi border
</commit_message>
<xml_diff>
--- a/car-count-test/car-count-test-cases.xlsx
+++ b/car-count-test/car-count-test-cases.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="246" uniqueCount="199">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="255" uniqueCount="204">
   <si>
     <t>description</t>
   </si>
@@ -623,6 +623,21 @@
   </si>
   <si>
     <t>updateTracks</t>
+  </si>
+  <si>
+    <t>occ006</t>
+  </si>
+  <si>
+    <t>extend rect to right or left border</t>
+  </si>
+  <si>
+    <t>occ007</t>
+  </si>
+  <si>
+    <t>track extension to left or right border</t>
+  </si>
+  <si>
+    <t>if track enters scene</t>
   </si>
 </sst>
 </file>
@@ -1054,13 +1069,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G70"/>
+  <dimension ref="A1:G72"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="5" ySplit="2" topLeftCell="H27" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="C45" sqref="C45"/>
+      <selection pane="bottomRight" activeCell="A28" sqref="A28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1470,29 +1485,31 @@
       <c r="A28" t="s">
         <v>146</v>
       </c>
-      <c r="B28" s="5" t="s">
-        <v>89</v>
+      <c r="B28" s="12" t="s">
+        <v>201</v>
       </c>
       <c r="C28" t="s">
-        <v>149</v>
+        <v>92</v>
       </c>
       <c r="D28" s="8" t="s">
-        <v>189</v>
-      </c>
-      <c r="E28" s="11"/>
+        <v>202</v>
+      </c>
+      <c r="E28" s="8" t="s">
+        <v>203</v>
+      </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>146</v>
       </c>
       <c r="B29" s="5" t="s">
-        <v>117</v>
+        <v>89</v>
       </c>
       <c r="C29" t="s">
-        <v>159</v>
+        <v>149</v>
       </c>
       <c r="D29" s="8" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="E29" s="11"/>
     </row>
@@ -1501,133 +1518,134 @@
         <v>146</v>
       </c>
       <c r="B30" s="5" t="s">
-        <v>133</v>
+        <v>117</v>
       </c>
       <c r="C30" t="s">
-        <v>152</v>
+        <v>159</v>
       </c>
       <c r="D30" s="8" t="s">
-        <v>191</v>
-      </c>
+        <v>190</v>
+      </c>
+      <c r="E30" s="11"/>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>146</v>
       </c>
       <c r="B31" s="5" t="s">
+        <v>133</v>
+      </c>
+      <c r="C31" t="s">
+        <v>152</v>
+      </c>
+      <c r="D31" s="8" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>146</v>
+      </c>
+      <c r="B32" s="5" t="s">
         <v>122</v>
       </c>
-      <c r="C31" t="s">
+      <c r="C32" t="s">
         <v>150</v>
       </c>
-      <c r="D31" s="8" t="s">
+      <c r="D32" s="8" t="s">
         <v>151</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B32" s="10"/>
-      <c r="D32" s="8"/>
-    </row>
-    <row r="33" spans="1:5" s="15" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="15" t="s">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>146</v>
+      </c>
+      <c r="B33" s="12" t="s">
+        <v>199</v>
+      </c>
+      <c r="C33" t="s">
+        <v>150</v>
+      </c>
+      <c r="D33" s="8" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B34" s="10"/>
+      <c r="D34" s="8"/>
+    </row>
+    <row r="35" spans="1:5" s="15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A35" s="15" t="s">
         <v>153</v>
       </c>
-      <c r="B33" s="14" t="s">
+      <c r="B35" s="14" t="s">
         <v>170</v>
       </c>
-      <c r="C33" s="15" t="s">
+      <c r="C35" s="15" t="s">
         <v>192</v>
       </c>
-      <c r="D33" s="16" t="s">
+      <c r="D35" s="16" t="s">
         <v>193</v>
       </c>
-      <c r="E33" s="16" t="s">
+      <c r="E35" s="16" t="s">
         <v>194</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A34" t="s">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
         <v>153</v>
       </c>
-      <c r="B34" s="5" t="s">
+      <c r="B36" s="5" t="s">
         <v>171</v>
       </c>
-      <c r="C34" t="s">
+      <c r="C36" t="s">
         <v>92</v>
       </c>
-      <c r="D34" s="8" t="s">
+      <c r="D36" s="8" t="s">
         <v>195</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="D35" s="8"/>
-    </row>
-    <row r="36" spans="1:5" s="15" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="15" t="s">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D37" s="8"/>
+    </row>
+    <row r="38" spans="1:5" s="15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A38" s="15" t="s">
         <v>88</v>
       </c>
-      <c r="B36" s="14" t="s">
+      <c r="B38" s="14" t="s">
         <v>173</v>
       </c>
-      <c r="C36" s="15" t="s">
+      <c r="C38" s="15" t="s">
         <v>92</v>
       </c>
-      <c r="D36" s="16" t="s">
+      <c r="D38" s="16" t="s">
         <v>129</v>
       </c>
-      <c r="E36" s="16" t="s">
+      <c r="E38" s="16" t="s">
         <v>112</v>
-      </c>
-    </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A37" t="s">
-        <v>88</v>
-      </c>
-      <c r="B37" s="12" t="s">
-        <v>196</v>
-      </c>
-      <c r="C37" t="s">
-        <v>148</v>
-      </c>
-      <c r="D37" s="8"/>
-    </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A38" t="s">
-        <v>88</v>
-      </c>
-      <c r="B38" s="5" t="s">
-        <v>176</v>
-      </c>
-      <c r="C38" t="s">
-        <v>124</v>
-      </c>
-      <c r="D38" s="8" t="s">
-        <v>126</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>88</v>
       </c>
-      <c r="B39" s="5" t="s">
-        <v>177</v>
+      <c r="B39" s="12" t="s">
+        <v>196</v>
       </c>
       <c r="C39" t="s">
-        <v>147</v>
-      </c>
-      <c r="D39" s="8" t="s">
-        <v>157</v>
-      </c>
+        <v>148</v>
+      </c>
+      <c r="D39" s="8"/>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>88</v>
       </c>
       <c r="B40" s="5" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="C40" t="s">
-        <v>132</v>
+        <v>124</v>
       </c>
       <c r="D40" s="8" t="s">
         <v>126</v>
@@ -1638,21 +1656,27 @@
         <v>88</v>
       </c>
       <c r="B41" s="5" t="s">
-        <v>172</v>
-      </c>
-      <c r="C41" s="8" t="s">
-        <v>185</v>
+        <v>177</v>
+      </c>
+      <c r="C41" t="s">
+        <v>147</v>
+      </c>
+      <c r="D41" s="8" t="s">
+        <v>157</v>
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>88</v>
       </c>
-      <c r="B42" s="12" t="s">
-        <v>186</v>
+      <c r="B42" s="5" t="s">
+        <v>178</v>
       </c>
       <c r="C42" t="s">
-        <v>154</v>
+        <v>132</v>
+      </c>
+      <c r="D42" s="8" t="s">
+        <v>126</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.25">
@@ -1660,16 +1684,10 @@
         <v>88</v>
       </c>
       <c r="B43" s="5" t="s">
-        <v>182</v>
-      </c>
-      <c r="C43" t="s">
-        <v>136</v>
-      </c>
-      <c r="D43" t="s">
-        <v>134</v>
-      </c>
-      <c r="E43" s="8" t="s">
-        <v>135</v>
+        <v>172</v>
+      </c>
+      <c r="C43" s="8" t="s">
+        <v>185</v>
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.25">
@@ -1677,97 +1695,91 @@
         <v>88</v>
       </c>
       <c r="B44" s="12" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="C44" t="s">
-        <v>155</v>
-      </c>
-      <c r="D44" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="45" spans="1:5" ht="75" x14ac:dyDescent="0.25">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>88</v>
       </c>
       <c r="B45" s="5" t="s">
+        <v>182</v>
+      </c>
+      <c r="C45" t="s">
+        <v>136</v>
+      </c>
+      <c r="D45" t="s">
+        <v>134</v>
+      </c>
+      <c r="E45" s="8" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>88</v>
+      </c>
+      <c r="B46" s="12" t="s">
+        <v>187</v>
+      </c>
+      <c r="C46" t="s">
+        <v>155</v>
+      </c>
+      <c r="D46" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" ht="75" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>88</v>
+      </c>
+      <c r="B47" s="5" t="s">
         <v>188</v>
       </c>
-      <c r="C45" t="s">
+      <c r="C47" t="s">
         <v>198</v>
       </c>
-      <c r="D45" t="s">
+      <c r="D47" t="s">
         <v>197</v>
       </c>
-      <c r="E45" s="8" t="s">
+      <c r="E47" s="8" t="s">
         <v>142</v>
       </c>
     </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B47" s="10"/>
-      <c r="D47" s="8"/>
-    </row>
-    <row r="48" spans="1:5" s="15" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A48" s="15" t="s">
+    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B49" s="10"/>
+      <c r="D49" s="8"/>
+    </row>
+    <row r="50" spans="1:6" s="15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A50" s="15" t="s">
         <v>174</v>
       </c>
-      <c r="B48" s="14" t="s">
+      <c r="B50" s="14" t="s">
         <v>184</v>
       </c>
-      <c r="C48" s="15" t="s">
+      <c r="C50" s="15" t="s">
         <v>138</v>
       </c>
-      <c r="D48" s="15" t="s">
+      <c r="D50" s="15" t="s">
         <v>139</v>
       </c>
-      <c r="E48" s="16"/>
-    </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A49" t="s">
-        <v>174</v>
-      </c>
-      <c r="B49" s="5" t="s">
-        <v>183</v>
-      </c>
-      <c r="C49" t="s">
-        <v>137</v>
-      </c>
-      <c r="D49" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A50" t="s">
-        <v>174</v>
-      </c>
-      <c r="B50" s="5" t="s">
-        <v>175</v>
-      </c>
-      <c r="C50" t="s">
-        <v>123</v>
-      </c>
-      <c r="D50" s="8" t="s">
-        <v>125</v>
-      </c>
-      <c r="E50" s="8" t="s">
-        <v>131</v>
-      </c>
+      <c r="E50" s="16"/>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>174</v>
       </c>
       <c r="B51" s="5" t="s">
-        <v>179</v>
+        <v>183</v>
       </c>
       <c r="C51" t="s">
-        <v>113</v>
+        <v>137</v>
       </c>
       <c r="D51" t="s">
-        <v>114</v>
-      </c>
-      <c r="E51" s="8" t="s">
-        <v>115</v>
+        <v>140</v>
       </c>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.25">
@@ -1775,13 +1787,16 @@
         <v>174</v>
       </c>
       <c r="B52" s="5" t="s">
-        <v>180</v>
+        <v>175</v>
       </c>
       <c r="C52" t="s">
-        <v>116</v>
-      </c>
-      <c r="D52" t="s">
-        <v>120</v>
+        <v>123</v>
+      </c>
+      <c r="D52" s="8" t="s">
+        <v>125</v>
+      </c>
+      <c r="E52" s="8" t="s">
+        <v>131</v>
       </c>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.25">
@@ -1789,38 +1804,44 @@
         <v>174</v>
       </c>
       <c r="B53" s="5" t="s">
+        <v>179</v>
+      </c>
+      <c r="C53" t="s">
+        <v>113</v>
+      </c>
+      <c r="D53" t="s">
+        <v>114</v>
+      </c>
+      <c r="E53" s="8" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
+        <v>174</v>
+      </c>
+      <c r="B54" s="5" t="s">
+        <v>180</v>
+      </c>
+      <c r="C54" t="s">
+        <v>116</v>
+      </c>
+      <c r="D54" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
+        <v>174</v>
+      </c>
+      <c r="B55" s="5" t="s">
         <v>181</v>
       </c>
-      <c r="C53" t="s">
+      <c r="C55" t="s">
         <v>119</v>
       </c>
-      <c r="D53" t="s">
+      <c r="D55" t="s">
         <v>121</v>
-      </c>
-    </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="C62" t="s">
-        <v>3</v>
-      </c>
-      <c r="D62" t="s">
-        <v>4</v>
-      </c>
-      <c r="E62" s="8" t="s">
-        <v>8</v>
-      </c>
-      <c r="F62" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="C63" t="s">
-        <v>3</v>
-      </c>
-      <c r="D63" t="s">
-        <v>5</v>
-      </c>
-      <c r="E63" s="8" t="s">
-        <v>9</v>
       </c>
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.25">
@@ -1828,34 +1849,59 @@
         <v>3</v>
       </c>
       <c r="D64" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="E64" s="8" t="s">
-        <v>10</v>
+        <v>8</v>
+      </c>
+      <c r="F64" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="65" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C65" t="s">
+        <v>3</v>
+      </c>
+      <c r="D65" t="s">
+        <v>5</v>
+      </c>
+      <c r="E65" s="8" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="66" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C66" t="s">
+        <v>3</v>
+      </c>
+      <c r="D66" t="s">
+        <v>6</v>
+      </c>
+      <c r="E66" s="8" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="68" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C68" t="s">
         <v>13</v>
       </c>
-      <c r="D66" t="s">
+      <c r="D68" t="s">
         <v>14</v>
       </c>
-      <c r="E66" s="8" t="s">
+      <c r="E68" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="F66" t="s">
+      <c r="F68" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="70" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C70" t="s">
+    <row r="72" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C72" t="s">
         <v>16</v>
       </c>
-      <c r="E70" s="8" t="s">
+      <c r="E72" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="F70" t="s">
+      <c r="F72" t="s">
         <v>21</v>
       </c>
     </row>

</xml_diff>

<commit_message>
gcc c++11 compatibility finished
</commit_message>
<xml_diff>
--- a/car-count-test/car-count-test-cases.xlsx
+++ b/car-count-test/car-count-test-cases.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="255" uniqueCount="204">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="255" uniqueCount="203">
   <si>
     <t>description</t>
   </si>
@@ -548,9 +548,6 @@
   </si>
   <si>
     <t>sce002</t>
-  </si>
-  <si>
-    <t>[fcn-scene]</t>
   </si>
   <si>
     <t>sce003</t>
@@ -708,7 +705,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -725,11 +722,20 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -763,6 +769,7 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -1072,10 +1079,10 @@
   <dimension ref="A1:G72"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="5" ySplit="2" topLeftCell="H27" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="5" ySplit="2" topLeftCell="H3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="A28" sqref="A28"/>
+      <selection pane="bottomRight" activeCell="C47" sqref="C47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1486,16 +1493,16 @@
         <v>146</v>
       </c>
       <c r="B28" s="12" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="C28" t="s">
         <v>92</v>
       </c>
       <c r="D28" s="8" t="s">
+        <v>201</v>
+      </c>
+      <c r="E28" s="8" t="s">
         <v>202</v>
-      </c>
-      <c r="E28" s="8" t="s">
-        <v>203</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
@@ -1509,7 +1516,7 @@
         <v>149</v>
       </c>
       <c r="D29" s="8" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="E29" s="11"/>
     </row>
@@ -1524,7 +1531,7 @@
         <v>159</v>
       </c>
       <c r="D30" s="8" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="E30" s="11"/>
     </row>
@@ -1539,7 +1546,7 @@
         <v>152</v>
       </c>
       <c r="D31" s="8" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
@@ -1561,13 +1568,13 @@
         <v>146</v>
       </c>
       <c r="B33" s="12" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="C33" t="s">
         <v>150</v>
       </c>
       <c r="D33" s="8" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
@@ -1582,13 +1589,13 @@
         <v>170</v>
       </c>
       <c r="C35" s="15" t="s">
+        <v>191</v>
+      </c>
+      <c r="D35" s="16" t="s">
         <v>192</v>
       </c>
-      <c r="D35" s="16" t="s">
+      <c r="E35" s="16" t="s">
         <v>193</v>
-      </c>
-      <c r="E35" s="16" t="s">
-        <v>194</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.25">
@@ -1602,7 +1609,7 @@
         <v>92</v>
       </c>
       <c r="D36" s="8" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.25">
@@ -1630,7 +1637,7 @@
         <v>88</v>
       </c>
       <c r="B39" s="12" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="C39" t="s">
         <v>148</v>
@@ -1642,7 +1649,7 @@
         <v>88</v>
       </c>
       <c r="B40" s="5" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="C40" t="s">
         <v>124</v>
@@ -1656,7 +1663,7 @@
         <v>88</v>
       </c>
       <c r="B41" s="5" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="C41" t="s">
         <v>147</v>
@@ -1670,7 +1677,7 @@
         <v>88</v>
       </c>
       <c r="B42" s="5" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="C42" t="s">
         <v>132</v>
@@ -1687,7 +1694,7 @@
         <v>172</v>
       </c>
       <c r="C43" s="8" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.25">
@@ -1695,7 +1702,7 @@
         <v>88</v>
       </c>
       <c r="B44" s="12" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="C44" t="s">
         <v>154</v>
@@ -1706,7 +1713,7 @@
         <v>88</v>
       </c>
       <c r="B45" s="5" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="C45" t="s">
         <v>136</v>
@@ -1723,7 +1730,7 @@
         <v>88</v>
       </c>
       <c r="B46" s="12" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="C46" t="s">
         <v>155</v>
@@ -1737,28 +1744,29 @@
         <v>88</v>
       </c>
       <c r="B47" s="5" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="C47" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="D47" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="E47" s="8" t="s">
         <v>142</v>
       </c>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A49" s="19"/>
       <c r="B49" s="10"/>
       <c r="D49" s="8"/>
     </row>
     <row r="50" spans="1:6" s="15" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A50" s="15" t="s">
-        <v>174</v>
+      <c r="A50" t="s">
+        <v>88</v>
       </c>
       <c r="B50" s="14" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="C50" s="15" t="s">
         <v>138</v>
@@ -1770,10 +1778,10 @@
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>174</v>
+        <v>88</v>
       </c>
       <c r="B51" s="5" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="C51" t="s">
         <v>137</v>
@@ -1784,10 +1792,10 @@
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
+        <v>88</v>
+      </c>
+      <c r="B52" s="5" t="s">
         <v>174</v>
-      </c>
-      <c r="B52" s="5" t="s">
-        <v>175</v>
       </c>
       <c r="C52" t="s">
         <v>123</v>
@@ -1801,10 +1809,10 @@
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>174</v>
+        <v>88</v>
       </c>
       <c r="B53" s="5" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="C53" t="s">
         <v>113</v>
@@ -1818,10 +1826,10 @@
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>174</v>
+        <v>88</v>
       </c>
       <c r="B54" s="5" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="C54" t="s">
         <v>116</v>
@@ -1832,10 +1840,10 @@
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>174</v>
+        <v>88</v>
       </c>
       <c r="B55" s="5" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="C55" t="s">
         <v>119</v>

</xml_diff>